<commit_message>
Save the transaction new 3 fields Serial Number Olimpo, Message ID and Channel flag (if comes from Olimpo other wise comes from X2X or MXS), for the transactions of TOTOLOTO, TOTOBOLA  AND INSTANTE LOTTERY. For this stage only the SON and SALEREP will be saved the field in the transaction for the Instant Lottery still needs to be completed.
</commit_message>
<xml_diff>
--- a/New Terminals/Sign-on/Sign-On.xlsx
+++ b/New Terminals/Sign-on/Sign-On.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\105864\Documents\Millennium\New Terminals\Sign-on\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F74100C-6255-49C4-A945-28919DCE4C4E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65C7EC8-7D6D-4CC6-B480-6FD4A9B083F6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A59DBA4C-956A-4B57-A1C8-C87C01DAE8BE}"/>
   </bookViews>
@@ -465,9 +465,6 @@
     <t>010001010111</t>
   </si>
   <si>
-    <t>Password de Administrador</t>
-  </si>
-  <si>
     <t xml:space="preserve">00 03 0F 22 </t>
   </si>
   <si>
@@ -758,12 +755,15 @@
       <t>X89 = Euromilhões</t>
     </r>
   </si>
+  <si>
+    <t>Password de Administrador/Gerente</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -818,13 +818,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1415,48 +1408,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
@@ -1469,13 +1420,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1512,77 +1457,125 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1994,8 +1987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4A5A7B-0DA8-401C-B426-04429DCC05B9}">
   <dimension ref="A2:S87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65:F65"/>
+    <sheetView tabSelected="1" topLeftCell="C43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2015,25 +2008,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="84" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
     </row>
     <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="2:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="37"/>
+      <c r="C4" s="87"/>
       <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="39"/>
+      <c r="F4" s="89"/>
       <c r="G4" s="12" t="s">
         <v>24</v>
       </c>
@@ -2052,8 +2045,8 @@
         <v>4</v>
       </c>
       <c r="D5" s="5"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="41"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="91"/>
     </row>
     <row r="6" spans="2:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="6">
@@ -2123,10 +2116,10 @@
       <c r="D8" s="9">
         <v>2</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="43"/>
+      <c r="F8" s="82"/>
       <c r="G8" s="12" t="s">
         <v>30</v>
       </c>
@@ -2150,10 +2143,10 @@
       <c r="D9" s="9">
         <v>1</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="35"/>
+      <c r="F9" s="73"/>
       <c r="G9" s="16" t="s">
         <v>39</v>
       </c>
@@ -2175,10 +2168,10 @@
       <c r="D10" s="9">
         <v>4</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E10" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="35"/>
+      <c r="F10" s="73"/>
       <c r="G10" s="19" t="s">
         <v>37</v>
       </c>
@@ -2202,10 +2195,10 @@
       <c r="D11" s="9">
         <v>2</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="35"/>
+      <c r="F11" s="73"/>
       <c r="G11" s="20" t="s">
         <v>38</v>
       </c>
@@ -2229,10 +2222,10 @@
       <c r="D12" s="9">
         <v>2</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="35"/>
+      <c r="F12" s="73"/>
       <c r="G12" s="19" t="s">
         <v>42</v>
       </c>
@@ -2256,10 +2249,10 @@
       <c r="D13" s="9">
         <v>8</v>
       </c>
-      <c r="E13" s="34" t="s">
+      <c r="E13" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="35"/>
+      <c r="F13" s="73"/>
       <c r="G13" s="20" t="s">
         <v>46</v>
       </c>
@@ -2283,10 +2276,10 @@
       <c r="D14" s="9">
         <v>8</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E14" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="35"/>
+      <c r="F14" s="73"/>
       <c r="G14" s="16" t="s">
         <v>48</v>
       </c>
@@ -2308,10 +2301,10 @@
       <c r="D15" s="9">
         <v>8</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="35"/>
+      <c r="F15" s="73"/>
       <c r="G15" s="19" t="s">
         <v>46</v>
       </c>
@@ -2335,10 +2328,10 @@
       <c r="D16" s="9">
         <v>8</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="E16" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="35"/>
+      <c r="F16" s="73"/>
       <c r="G16" s="19" t="s">
         <v>46</v>
       </c>
@@ -2362,10 +2355,10 @@
       <c r="D17" s="9">
         <v>8</v>
       </c>
-      <c r="E17" s="34" t="s">
+      <c r="E17" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="35"/>
+      <c r="F17" s="73"/>
       <c r="G17" s="19" t="s">
         <v>46</v>
       </c>
@@ -2389,10 +2382,10 @@
       <c r="D18" s="9">
         <v>8</v>
       </c>
-      <c r="E18" s="34" t="s">
+      <c r="E18" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="35"/>
+      <c r="F18" s="73"/>
       <c r="G18" s="19" t="s">
         <v>46</v>
       </c>
@@ -2416,10 +2409,10 @@
       <c r="D19" s="9">
         <v>4</v>
       </c>
-      <c r="E19" s="34" t="s">
+      <c r="E19" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="35"/>
+      <c r="F19" s="73"/>
       <c r="G19" s="19" t="s">
         <v>50</v>
       </c>
@@ -2443,10 +2436,10 @@
       <c r="D20" s="9">
         <v>4</v>
       </c>
-      <c r="E20" s="34" t="s">
+      <c r="E20" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="35"/>
+      <c r="F20" s="73"/>
       <c r="G20" s="16" t="s">
         <v>51</v>
       </c>
@@ -2470,10 +2463,10 @@
       <c r="D21" s="9">
         <v>4</v>
       </c>
-      <c r="E21" s="34" t="s">
+      <c r="E21" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="35"/>
+      <c r="F21" s="73"/>
       <c r="G21" s="16" t="s">
         <v>52</v>
       </c>
@@ -2497,10 +2490,10 @@
       <c r="D22" s="9">
         <v>4</v>
       </c>
-      <c r="E22" s="34" t="s">
+      <c r="E22" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="35"/>
+      <c r="F22" s="73"/>
       <c r="G22" s="16" t="s">
         <v>50</v>
       </c>
@@ -2524,10 +2517,10 @@
       <c r="D23" s="9">
         <v>4</v>
       </c>
-      <c r="E23" s="34" t="s">
+      <c r="E23" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="35"/>
+      <c r="F23" s="73"/>
       <c r="G23" s="24" t="s">
         <v>54</v>
       </c>
@@ -2551,10 +2544,10 @@
       <c r="D24" s="9">
         <v>4</v>
       </c>
-      <c r="E24" s="34" t="s">
+      <c r="E24" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="35"/>
+      <c r="F24" s="73"/>
       <c r="G24" s="19" t="s">
         <v>53</v>
       </c>
@@ -2578,10 +2571,10 @@
       <c r="D25" s="9">
         <v>4</v>
       </c>
-      <c r="E25" s="34" t="s">
+      <c r="E25" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="35"/>
+      <c r="F25" s="73"/>
       <c r="G25" s="19" t="s">
         <v>53</v>
       </c>
@@ -2605,10 +2598,10 @@
       <c r="D26" s="9">
         <v>4</v>
       </c>
-      <c r="E26" s="34" t="s">
+      <c r="E26" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="35"/>
+      <c r="F26" s="73"/>
       <c r="G26" s="19" t="s">
         <v>50</v>
       </c>
@@ -2632,10 +2625,10 @@
       <c r="D27" s="9">
         <v>4</v>
       </c>
-      <c r="E27" s="34" t="s">
+      <c r="E27" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="F27" s="35"/>
+      <c r="F27" s="73"/>
       <c r="G27" s="19" t="s">
         <v>50</v>
       </c>
@@ -2659,10 +2652,10 @@
       <c r="D28" s="9">
         <v>4</v>
       </c>
-      <c r="E28" s="34" t="s">
+      <c r="E28" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="F28" s="35"/>
+      <c r="F28" s="73"/>
       <c r="G28" s="19" t="s">
         <v>50</v>
       </c>
@@ -2686,10 +2679,10 @@
       <c r="D29" s="9">
         <v>4</v>
       </c>
-      <c r="E29" s="34" t="s">
+      <c r="E29" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="35"/>
+      <c r="F29" s="73"/>
       <c r="G29" s="19" t="s">
         <v>50</v>
       </c>
@@ -2713,10 +2706,10 @@
       <c r="D30" s="11">
         <v>4</v>
       </c>
-      <c r="E30" s="44" t="s">
+      <c r="E30" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="F30" s="45"/>
+      <c r="F30" s="75"/>
       <c r="G30" s="19" t="s">
         <v>50</v>
       </c>
@@ -2732,12 +2725,12 @@
     </row>
     <row r="31" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="34" spans="2:19" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B34" s="48" t="s">
+      <c r="B34" s="34" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="35" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="49"/>
+      <c r="B35" s="35"/>
     </row>
     <row r="36" spans="2:19" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B36" s="28" t="s">
@@ -2843,10 +2836,10 @@
       <c r="D40" s="9">
         <v>2</v>
       </c>
-      <c r="E40" s="42" t="s">
+      <c r="E40" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="F40" s="43"/>
+      <c r="F40" s="82"/>
       <c r="G40" s="16" t="s">
         <v>82</v>
       </c>
@@ -2867,10 +2860,10 @@
       <c r="D41" s="9">
         <v>3</v>
       </c>
-      <c r="E41" s="34" t="s">
+      <c r="E41" s="76" t="s">
         <v>63</v>
       </c>
-      <c r="F41" s="35"/>
+      <c r="F41" s="73"/>
       <c r="G41" s="19" t="s">
         <v>85</v>
       </c>
@@ -2880,7 +2873,7 @@
       <c r="I41" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="J41" s="53" t="s">
+      <c r="J41" s="38" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2894,10 +2887,10 @@
       <c r="D42" s="9">
         <v>2</v>
       </c>
-      <c r="E42" s="34" t="s">
+      <c r="E42" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="F42" s="35"/>
+      <c r="F42" s="73"/>
       <c r="G42" s="19" t="s">
         <v>89</v>
       </c>
@@ -2910,14 +2903,14 @@
       <c r="J42" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="L42" s="54"/>
-      <c r="M42" s="54"/>
-      <c r="N42" s="54"/>
-      <c r="O42" s="54"/>
-      <c r="P42" s="54"/>
-      <c r="Q42" s="54"/>
-      <c r="R42" s="54"/>
-      <c r="S42" s="54"/>
+      <c r="L42" s="78"/>
+      <c r="M42" s="78"/>
+      <c r="N42" s="78"/>
+      <c r="O42" s="78"/>
+      <c r="P42" s="78"/>
+      <c r="Q42" s="78"/>
+      <c r="R42" s="78"/>
+      <c r="S42" s="78"/>
     </row>
     <row r="43" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B43" s="8">
@@ -2929,10 +2922,10 @@
       <c r="D43" s="9">
         <v>2</v>
       </c>
-      <c r="E43" s="34" t="s">
+      <c r="E43" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="F43" s="35"/>
+      <c r="F43" s="73"/>
       <c r="G43" s="16" t="s">
         <v>93</v>
       </c>
@@ -2956,20 +2949,20 @@
       <c r="D44" s="9">
         <v>1</v>
       </c>
-      <c r="E44" s="34" t="s">
+      <c r="E44" s="76" t="s">
         <v>66</v>
       </c>
-      <c r="F44" s="35"/>
-      <c r="G44" s="82" t="s">
+      <c r="F44" s="73"/>
+      <c r="G44" s="62" t="s">
         <v>96</v>
       </c>
-      <c r="H44" s="82" t="s">
+      <c r="H44" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="I44" s="82" t="s">
+      <c r="I44" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="J44" s="83" t="s">
+      <c r="J44" s="63" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2983,10 +2976,10 @@
       <c r="D45" s="9">
         <v>2</v>
       </c>
-      <c r="E45" s="34" t="s">
+      <c r="E45" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="F45" s="35"/>
+      <c r="F45" s="73"/>
       <c r="G45" s="12" t="s">
         <v>100</v>
       </c>
@@ -2996,7 +2989,7 @@
       <c r="I45" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="J45" s="55" t="s">
+      <c r="J45" s="39" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3010,10 +3003,10 @@
       <c r="D46" s="9">
         <v>1</v>
       </c>
-      <c r="E46" s="34" t="s">
+      <c r="E46" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="F46" s="35"/>
+      <c r="F46" s="73"/>
       <c r="G46" s="19" t="s">
         <v>104</v>
       </c>
@@ -3023,7 +3016,7 @@
       <c r="I46" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="J46" s="53" t="s">
+      <c r="J46" s="38" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3037,10 +3030,10 @@
       <c r="D47" s="9">
         <v>4</v>
       </c>
-      <c r="E47" s="34" t="s">
+      <c r="E47" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="35"/>
+      <c r="F47" s="73"/>
       <c r="G47" s="18" t="s">
         <v>37</v>
       </c>
@@ -3064,26 +3057,26 @@
       <c r="D48" s="9">
         <v>1</v>
       </c>
-      <c r="E48" s="51" t="s">
+      <c r="E48" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="F48" s="51" t="s">
+      <c r="F48" s="37" t="s">
         <v>70</v>
       </c>
       <c r="G48" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="H48" s="56" t="s">
+      <c r="H48" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="I48" s="56" t="s">
+      <c r="I48" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="J48" s="57" t="s">
+      <c r="J48" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="K48" s="58"/>
-      <c r="L48" s="59" t="s">
+      <c r="K48" s="42"/>
+      <c r="L48" s="43" t="s">
         <v>114</v>
       </c>
     </row>
@@ -3097,10 +3090,10 @@
       <c r="D49" s="9">
         <v>2</v>
       </c>
-      <c r="E49" s="34" t="s">
+      <c r="E49" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="F49" s="35"/>
+      <c r="F49" s="73"/>
       <c r="G49" s="19" t="s">
         <v>116</v>
       </c>
@@ -3110,7 +3103,7 @@
       <c r="I49" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="J49" s="60" t="s">
+      <c r="J49" s="44" t="s">
         <v>119</v>
       </c>
     </row>
@@ -3124,18 +3117,18 @@
       <c r="D50" s="9">
         <v>2</v>
       </c>
-      <c r="E50" s="34" t="s">
+      <c r="E50" s="76" t="s">
         <v>72</v>
       </c>
-      <c r="F50" s="35"/>
+      <c r="F50" s="73"/>
       <c r="G50" s="16" t="s">
         <v>120</v>
       </c>
       <c r="H50" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I50" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="51" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3148,18 +3141,18 @@
       <c r="D51" s="9">
         <v>2</v>
       </c>
-      <c r="E51" s="34" t="s">
+      <c r="E51" s="76" t="s">
         <v>73</v>
       </c>
-      <c r="F51" s="35"/>
+      <c r="F51" s="73"/>
       <c r="G51" s="16" t="s">
         <v>120</v>
       </c>
       <c r="H51" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I51" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="52" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3172,10 +3165,10 @@
       <c r="D52" s="9">
         <v>2</v>
       </c>
-      <c r="E52" s="34" t="s">
+      <c r="E52" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="F52" s="35"/>
+      <c r="F52" s="73"/>
       <c r="G52" s="16" t="s">
         <v>38</v>
       </c>
@@ -3199,10 +3192,10 @@
       <c r="D53" s="9">
         <v>4</v>
       </c>
-      <c r="E53" s="34" t="s">
+      <c r="E53" s="76" t="s">
         <v>75</v>
       </c>
-      <c r="F53" s="35"/>
+      <c r="F53" s="73"/>
       <c r="G53" s="19" t="s">
         <v>50</v>
       </c>
@@ -3213,7 +3206,7 @@
         <v>47</v>
       </c>
       <c r="J53" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="54" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3226,21 +3219,21 @@
       <c r="D54" s="9">
         <v>4</v>
       </c>
-      <c r="E54" s="34" t="s">
+      <c r="E54" s="76" t="s">
         <v>76</v>
       </c>
-      <c r="F54" s="35"/>
+      <c r="F54" s="73"/>
       <c r="G54" s="18" t="s">
         <v>121</v>
       </c>
       <c r="H54" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I54" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J54" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="55" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3253,10 +3246,10 @@
       <c r="D55" s="9">
         <v>2</v>
       </c>
-      <c r="E55" s="34" t="s">
+      <c r="E55" s="76" t="s">
         <v>77</v>
       </c>
-      <c r="F55" s="35"/>
+      <c r="F55" s="73"/>
       <c r="G55" s="18" t="s">
         <v>122</v>
       </c>
@@ -3267,7 +3260,7 @@
         <v>123</v>
       </c>
       <c r="J55" s="18" t="s">
-        <v>125</v>
+        <v>218</v>
       </c>
     </row>
     <row r="56" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3280,10 +3273,10 @@
       <c r="D56" s="9">
         <v>2</v>
       </c>
-      <c r="E56" s="34" t="s">
+      <c r="E56" s="76" t="s">
         <v>78</v>
       </c>
-      <c r="F56" s="35"/>
+      <c r="F56" s="73"/>
       <c r="G56" s="19" t="s">
         <v>38</v>
       </c>
@@ -3293,8 +3286,8 @@
       <c r="I56" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="J56" s="53" t="s">
-        <v>128</v>
+      <c r="J56" s="38" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="57" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3307,10 +3300,10 @@
       <c r="D57" s="9">
         <v>8</v>
       </c>
-      <c r="E57" s="34" t="s">
+      <c r="E57" s="76" t="s">
         <v>78</v>
       </c>
-      <c r="F57" s="35"/>
+      <c r="F57" s="73"/>
       <c r="G57" s="19" t="s">
         <v>46</v>
       </c>
@@ -3320,11 +3313,11 @@
       <c r="I57" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="J57" s="53" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J57" s="38" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B58" s="8">
         <v>49</v>
       </c>
@@ -3334,24 +3327,24 @@
       <c r="D58" s="9">
         <v>4</v>
       </c>
-      <c r="E58" s="34" t="s">
+      <c r="E58" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="F58" s="35"/>
+      <c r="F58" s="73"/>
       <c r="G58" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="H58" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="H58" s="19" t="s">
-        <v>127</v>
-      </c>
       <c r="I58" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="J58" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="J58" s="15" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="59" spans="1:16" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B59" s="8">
         <v>53</v>
       </c>
@@ -3361,401 +3354,401 @@
       <c r="D59" s="9">
         <v>4</v>
       </c>
-      <c r="E59" s="34" t="s">
+      <c r="E59" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="F59" s="35"/>
+      <c r="F59" s="73"/>
       <c r="G59" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H59" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="I59" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="H59" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="I59" s="19" t="s">
-        <v>132</v>
-      </c>
       <c r="J59" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="61" spans="1:16" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B61" s="73" t="s">
-        <v>152</v>
-      </c>
-      <c r="C61" s="73"/>
-      <c r="D61" s="73"/>
-      <c r="E61" s="73"/>
-      <c r="F61" s="73"/>
-      <c r="L61" s="76" t="s">
+      <c r="B61" s="79" t="s">
+        <v>151</v>
+      </c>
+      <c r="C61" s="79"/>
+      <c r="D61" s="79"/>
+      <c r="E61" s="79"/>
+      <c r="F61" s="79"/>
+      <c r="L61" s="56" t="s">
+        <v>167</v>
+      </c>
+      <c r="M61" s="57" t="s">
         <v>168</v>
       </c>
-      <c r="M61" s="77" t="s">
+      <c r="N61" s="57" t="s">
         <v>169</v>
       </c>
-      <c r="N61" s="77" t="s">
+      <c r="O61" s="57" t="s">
         <v>170</v>
       </c>
-      <c r="O61" s="77" t="s">
+      <c r="P61" s="58" t="s">
         <v>171</v>
       </c>
-      <c r="P61" s="78" t="s">
+    </row>
+    <row r="62" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B62" s="45">
+        <v>57</v>
+      </c>
+      <c r="C62" s="46">
+        <v>57</v>
+      </c>
+      <c r="D62" s="46">
+        <v>1</v>
+      </c>
+      <c r="E62" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="F62" s="52"/>
+      <c r="G62" s="54" t="s">
+        <v>157</v>
+      </c>
+      <c r="H62" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="I62" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="J62" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="L62" s="68">
+        <v>1</v>
+      </c>
+      <c r="M62" s="69" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="62" spans="1:16" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B62" s="61">
-        <v>57</v>
-      </c>
-      <c r="C62" s="62">
-        <v>57</v>
-      </c>
-      <c r="D62" s="62">
+      <c r="N62" s="70">
+        <v>17</v>
+      </c>
+      <c r="O62" s="70">
         <v>1</v>
       </c>
-      <c r="E62" s="69" t="s">
+      <c r="P62" s="71" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B63" s="47">
+        <v>58</v>
+      </c>
+      <c r="C63" s="48">
+        <v>58</v>
+      </c>
+      <c r="D63" s="48">
+        <v>1</v>
+      </c>
+      <c r="E63" s="53" t="s">
         <v>134</v>
-      </c>
-      <c r="F62" s="70"/>
-      <c r="G62" s="74" t="s">
-        <v>158</v>
-      </c>
-      <c r="H62" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="I62" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="J62" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="L62" s="88">
-        <v>1</v>
-      </c>
-      <c r="M62" s="89" t="s">
-        <v>173</v>
-      </c>
-      <c r="N62" s="90">
-        <v>17</v>
-      </c>
-      <c r="O62" s="90">
-        <v>1</v>
-      </c>
-      <c r="P62" s="91" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B63" s="63">
-        <v>58</v>
-      </c>
-      <c r="C63" s="64">
-        <v>58</v>
-      </c>
-      <c r="D63" s="64">
-        <v>1</v>
-      </c>
-      <c r="E63" s="71" t="s">
-        <v>135</v>
       </c>
       <c r="F63" s="27"/>
       <c r="G63" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="H63" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="I63" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="H63" s="16" t="s">
+      <c r="J63" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="I63" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="J63" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="L63" s="65">
+      <c r="L63" s="49">
         <v>2</v>
       </c>
-      <c r="M63" s="79" t="s">
+      <c r="M63" s="59" t="s">
+        <v>174</v>
+      </c>
+      <c r="N63" s="50">
+        <v>19</v>
+      </c>
+      <c r="O63" s="50">
+        <v>2</v>
+      </c>
+      <c r="P63" s="37" t="s">
         <v>175</v>
-      </c>
-      <c r="N63" s="66">
-        <v>19</v>
-      </c>
-      <c r="O63" s="66">
-        <v>2</v>
-      </c>
-      <c r="P63" s="51" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="64" spans="1:16" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="12">
         <v>59</v>
       </c>
-      <c r="B64" s="65" t="s">
+      <c r="B64" s="49" t="s">
+        <v>135</v>
+      </c>
+      <c r="C64" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="C64" s="66" t="s">
+      <c r="D64" s="50">
+        <v>1</v>
+      </c>
+      <c r="E64" s="50" t="s">
         <v>137</v>
       </c>
-      <c r="D64" s="66">
+      <c r="F64" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="G64" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="H64" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="I64" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="J64" s="67" t="s">
+        <v>217</v>
+      </c>
+      <c r="L64" s="49">
+        <v>3</v>
+      </c>
+      <c r="M64" s="59" t="s">
+        <v>176</v>
+      </c>
+      <c r="N64" s="50">
+        <v>2</v>
+      </c>
+      <c r="O64" s="50">
         <v>1</v>
       </c>
-      <c r="E64" s="66" t="s">
-        <v>138</v>
-      </c>
-      <c r="F64" s="51" t="s">
-        <v>139</v>
-      </c>
-      <c r="G64" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="H64" s="25" t="s">
-        <v>214</v>
-      </c>
-      <c r="I64" s="25" t="s">
-        <v>217</v>
-      </c>
-      <c r="J64" s="87" t="s">
-        <v>218</v>
-      </c>
-      <c r="L64" s="65">
-        <v>3</v>
-      </c>
-      <c r="M64" s="79" t="s">
+      <c r="P64" s="37" t="s">
         <v>177</v>
-      </c>
-      <c r="N64" s="66">
-        <v>2</v>
-      </c>
-      <c r="O64" s="66">
-        <v>1</v>
-      </c>
-      <c r="P64" s="51" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="65" spans="1:16" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="B65" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="C65" s="50" t="s">
+        <v>140</v>
+      </c>
+      <c r="D65" s="50">
+        <v>2</v>
+      </c>
+      <c r="E65" s="72" t="s">
+        <v>141</v>
+      </c>
+      <c r="F65" s="73"/>
+      <c r="G65" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="B65" s="65" t="s">
-        <v>140</v>
-      </c>
-      <c r="C65" s="66" t="s">
-        <v>141</v>
-      </c>
-      <c r="D65" s="66">
-        <v>2</v>
-      </c>
-      <c r="E65" s="68" t="s">
-        <v>142</v>
-      </c>
-      <c r="F65" s="35"/>
-      <c r="G65" s="16" t="s">
+      <c r="H65" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="H65" s="16" t="s">
+      <c r="I65" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="I65" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="J65" s="50" t="s">
-        <v>191</v>
-      </c>
-      <c r="L65" s="65">
+      <c r="J65" s="36" t="s">
+        <v>190</v>
+      </c>
+      <c r="L65" s="49">
         <v>4</v>
       </c>
-      <c r="M65" s="79" t="s">
+      <c r="M65" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="N65" s="50">
+        <v>4</v>
+      </c>
+      <c r="O65" s="50">
+        <v>1</v>
+      </c>
+      <c r="P65" s="37" t="s">
         <v>179</v>
-      </c>
-      <c r="N65" s="66">
-        <v>4</v>
-      </c>
-      <c r="O65" s="66">
-        <v>1</v>
-      </c>
-      <c r="P65" s="51" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="66" spans="1:16" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="B66" s="65" t="s">
+        <v>191</v>
+      </c>
+      <c r="B66" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="C66" s="50" t="s">
         <v>143</v>
       </c>
-      <c r="C66" s="66" t="s">
+      <c r="D66" s="50">
+        <v>2</v>
+      </c>
+      <c r="E66" s="72" t="s">
         <v>144</v>
       </c>
-      <c r="D66" s="66">
-        <v>2</v>
-      </c>
-      <c r="E66" s="68" t="s">
-        <v>145</v>
-      </c>
-      <c r="F66" s="35"/>
+      <c r="F66" s="73"/>
       <c r="G66" s="16" t="s">
         <v>120</v>
       </c>
       <c r="H66" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I66" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J66" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="L66" s="65">
+        <v>194</v>
+      </c>
+      <c r="L66" s="49">
         <v>5</v>
       </c>
-      <c r="M66" s="79" t="s">
+      <c r="M66" s="59" t="s">
+        <v>180</v>
+      </c>
+      <c r="N66" s="50">
+        <v>1</v>
+      </c>
+      <c r="O66" s="50">
+        <v>3</v>
+      </c>
+      <c r="P66" s="37" t="s">
         <v>181</v>
-      </c>
-      <c r="N66" s="66">
-        <v>1</v>
-      </c>
-      <c r="O66" s="66">
-        <v>3</v>
-      </c>
-      <c r="P66" s="51" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="67" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A67" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="B67" s="65" t="s">
+        <v>192</v>
+      </c>
+      <c r="B67" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="C67" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="C67" s="66" t="s">
+      <c r="D67" s="50">
+        <v>2</v>
+      </c>
+      <c r="E67" s="72" t="s">
         <v>147</v>
       </c>
-      <c r="D67" s="66">
-        <v>2</v>
-      </c>
-      <c r="E67" s="68" t="s">
-        <v>148</v>
-      </c>
-      <c r="F67" s="35"/>
+      <c r="F67" s="73"/>
       <c r="G67" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="H67" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="I67" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="H67" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="I67" s="16" t="s">
-        <v>197</v>
-      </c>
       <c r="J67" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="L67" s="65">
+        <v>194</v>
+      </c>
+      <c r="L67" s="49">
         <v>6</v>
       </c>
-      <c r="M67" s="79" t="s">
+      <c r="M67" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="N67" s="50">
+        <v>1</v>
+      </c>
+      <c r="O67" s="50">
+        <v>4</v>
+      </c>
+      <c r="P67" s="37" t="s">
         <v>183</v>
-      </c>
-      <c r="N67" s="66">
-        <v>1</v>
-      </c>
-      <c r="O67" s="66">
-        <v>4</v>
-      </c>
-      <c r="P67" s="51" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="68" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="B68" s="63" t="s">
+        <v>193</v>
+      </c>
+      <c r="B68" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="C68" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="C68" s="64" t="s">
+      <c r="D68" s="48">
+        <v>2</v>
+      </c>
+      <c r="E68" s="74" t="s">
         <v>150</v>
       </c>
-      <c r="D68" s="64">
-        <v>2</v>
-      </c>
-      <c r="E68" s="67" t="s">
-        <v>151</v>
-      </c>
-      <c r="F68" s="45"/>
+      <c r="F68" s="75"/>
       <c r="G68" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="H68" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="I68" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="H68" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="I68" s="16" t="s">
-        <v>200</v>
-      </c>
       <c r="J68" s="12"/>
-      <c r="L68" s="65">
+      <c r="L68" s="49">
         <v>7</v>
       </c>
-      <c r="M68" s="79" t="s">
+      <c r="M68" s="59" t="s">
+        <v>184</v>
+      </c>
+      <c r="N68" s="50">
+        <v>16</v>
+      </c>
+      <c r="O68" s="50">
+        <v>1</v>
+      </c>
+      <c r="P68" s="37" t="s">
         <v>185</v>
-      </c>
-      <c r="N68" s="66">
-        <v>16</v>
-      </c>
-      <c r="O68" s="66">
-        <v>1</v>
-      </c>
-      <c r="P68" s="51" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="69" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H69" s="12"/>
       <c r="I69" s="12"/>
       <c r="J69" s="12"/>
-      <c r="L69" s="65">
+      <c r="L69" s="49">
         <v>8</v>
       </c>
-      <c r="M69" s="79" t="s">
+      <c r="M69" s="59" t="s">
+        <v>186</v>
+      </c>
+      <c r="N69" s="50">
+        <v>16</v>
+      </c>
+      <c r="O69" s="50">
+        <v>2</v>
+      </c>
+      <c r="P69" s="37" t="s">
         <v>187</v>
       </c>
-      <c r="N69" s="66">
-        <v>16</v>
-      </c>
-      <c r="O69" s="66">
+    </row>
+    <row r="70" spans="1:16" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="65" t="s">
+        <v>210</v>
+      </c>
+      <c r="B70" s="66" t="s">
+        <v>209</v>
+      </c>
+      <c r="G70" s="66" t="s">
+        <v>211</v>
+      </c>
+      <c r="L70" s="47">
+        <v>9</v>
+      </c>
+      <c r="M70" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="N70" s="48">
         <v>2</v>
       </c>
-      <c r="P69" s="51" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="85" t="s">
-        <v>211</v>
-      </c>
-      <c r="B70" s="86" t="s">
-        <v>210</v>
-      </c>
-      <c r="G70" s="86" t="s">
-        <v>212</v>
-      </c>
-      <c r="L70" s="63">
-        <v>9</v>
-      </c>
-      <c r="M70" s="80" t="s">
+      <c r="O70" s="48">
+        <v>3</v>
+      </c>
+      <c r="P70" s="61" t="s">
         <v>189</v>
-      </c>
-      <c r="N70" s="64">
-        <v>2</v>
-      </c>
-      <c r="O70" s="64">
-        <v>3</v>
-      </c>
-      <c r="P70" s="81" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="71" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -3763,23 +3756,23 @@
       <c r="A72" s="12">
         <v>68</v>
       </c>
-      <c r="B72" s="65" t="s">
+      <c r="B72" s="49" t="s">
+        <v>135</v>
+      </c>
+      <c r="C72" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="C72" s="66" t="s">
+      <c r="D72" s="50">
+        <v>1</v>
+      </c>
+      <c r="E72" s="50" t="s">
         <v>137</v>
       </c>
-      <c r="D72" s="66">
-        <v>1</v>
-      </c>
-      <c r="E72" s="66" t="s">
+      <c r="F72" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="F72" s="51" t="s">
-        <v>139</v>
-      </c>
       <c r="G72" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H72" s="12">
         <v>1</v>
@@ -3787,216 +3780,246 @@
       <c r="I72" s="12">
         <v>1</v>
       </c>
-      <c r="L72" s="72" t="s">
-        <v>215</v>
-      </c>
-      <c r="M72" s="72"/>
-      <c r="N72" s="72"/>
+      <c r="L72" s="80" t="s">
+        <v>214</v>
+      </c>
+      <c r="M72" s="80"/>
+      <c r="N72" s="80"/>
     </row>
     <row r="73" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="B73" s="65" t="s">
+        <v>201</v>
+      </c>
+      <c r="B73" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="C73" s="50" t="s">
         <v>140</v>
       </c>
-      <c r="C73" s="66" t="s">
+      <c r="D73" s="50">
+        <v>2</v>
+      </c>
+      <c r="E73" s="72" t="s">
         <v>141</v>
       </c>
-      <c r="D73" s="66">
-        <v>2</v>
-      </c>
-      <c r="E73" s="68" t="s">
-        <v>142</v>
-      </c>
-      <c r="F73" s="35"/>
-      <c r="G73" s="75"/>
-      <c r="L73" s="72" t="s">
-        <v>216</v>
-      </c>
-      <c r="M73" s="72"/>
+      <c r="F73" s="73"/>
+      <c r="G73" s="55"/>
+      <c r="L73" s="80" t="s">
+        <v>215</v>
+      </c>
+      <c r="M73" s="80"/>
     </row>
     <row r="74" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="B74" s="65" t="s">
+        <v>202</v>
+      </c>
+      <c r="B74" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="C74" s="50" t="s">
         <v>143</v>
       </c>
-      <c r="C74" s="66" t="s">
+      <c r="D74" s="50">
+        <v>2</v>
+      </c>
+      <c r="E74" s="64" t="s">
         <v>144</v>
       </c>
-      <c r="D74" s="66">
-        <v>2</v>
-      </c>
-      <c r="E74" s="84" t="s">
-        <v>145</v>
-      </c>
       <c r="F74" s="26"/>
-      <c r="G74" s="75"/>
+      <c r="G74" s="55"/>
     </row>
     <row r="75" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="B75" s="65" t="s">
+        <v>203</v>
+      </c>
+      <c r="B75" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="C75" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="C75" s="66" t="s">
+      <c r="D75" s="50">
+        <v>2</v>
+      </c>
+      <c r="E75" s="64" t="s">
         <v>147</v>
       </c>
-      <c r="D75" s="66">
-        <v>2</v>
-      </c>
-      <c r="E75" s="84" t="s">
-        <v>148</v>
-      </c>
       <c r="F75" s="26"/>
-      <c r="G75" s="75"/>
+      <c r="G75" s="55"/>
     </row>
     <row r="76" spans="1:16" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="B76" s="63" t="s">
+        <v>204</v>
+      </c>
+      <c r="B76" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="C76" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="C76" s="64" t="s">
+      <c r="D76" s="48">
+        <v>2</v>
+      </c>
+      <c r="E76" s="53" t="s">
         <v>150</v>
       </c>
-      <c r="D76" s="64">
-        <v>2</v>
-      </c>
-      <c r="E76" s="71" t="s">
-        <v>151</v>
-      </c>
       <c r="F76" s="27"/>
-      <c r="G76" s="75"/>
+      <c r="G76" s="55"/>
     </row>
     <row r="77" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="78" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="12">
         <v>77</v>
       </c>
-      <c r="B78" s="65" t="s">
+      <c r="B78" s="49" t="s">
+        <v>135</v>
+      </c>
+      <c r="C78" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="C78" s="66" t="s">
+      <c r="D78" s="50">
+        <v>1</v>
+      </c>
+      <c r="E78" s="50" t="s">
         <v>137</v>
       </c>
-      <c r="D78" s="66">
-        <v>1</v>
-      </c>
-      <c r="E78" s="66" t="s">
+      <c r="F78" s="37" t="s">
         <v>138</v>
-      </c>
-      <c r="F78" s="51" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="79" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="B79" s="65" t="s">
+        <v>205</v>
+      </c>
+      <c r="B79" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="C79" s="50" t="s">
         <v>140</v>
       </c>
-      <c r="C79" s="66" t="s">
+      <c r="D79" s="50">
+        <v>2</v>
+      </c>
+      <c r="E79" s="64" t="s">
         <v>141</v>
-      </c>
-      <c r="D79" s="66">
-        <v>2</v>
-      </c>
-      <c r="E79" s="84" t="s">
-        <v>142</v>
       </c>
       <c r="F79" s="26"/>
     </row>
     <row r="80" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="B80" s="65" t="s">
+        <v>206</v>
+      </c>
+      <c r="B80" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="C80" s="50" t="s">
         <v>143</v>
       </c>
-      <c r="C80" s="66" t="s">
+      <c r="D80" s="50">
+        <v>2</v>
+      </c>
+      <c r="E80" s="64" t="s">
         <v>144</v>
-      </c>
-      <c r="D80" s="66">
-        <v>2</v>
-      </c>
-      <c r="E80" s="84" t="s">
-        <v>145</v>
       </c>
       <c r="F80" s="26"/>
     </row>
     <row r="81" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="B81" s="65" t="s">
+        <v>207</v>
+      </c>
+      <c r="B81" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="C81" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="C81" s="66" t="s">
+      <c r="D81" s="50">
+        <v>2</v>
+      </c>
+      <c r="E81" s="64" t="s">
         <v>147</v>
-      </c>
-      <c r="D81" s="66">
-        <v>2</v>
-      </c>
-      <c r="E81" s="84" t="s">
-        <v>148</v>
       </c>
       <c r="F81" s="26"/>
     </row>
     <row r="82" spans="1:6" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="B82" s="63" t="s">
+        <v>208</v>
+      </c>
+      <c r="B82" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="C82" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="C82" s="64" t="s">
+      <c r="D82" s="48">
+        <v>2</v>
+      </c>
+      <c r="E82" s="53" t="s">
         <v>150</v>
-      </c>
-      <c r="D82" s="64">
-        <v>2</v>
-      </c>
-      <c r="E82" s="71" t="s">
-        <v>151</v>
       </c>
       <c r="F82" s="27"/>
     </row>
     <row r="83" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B85" s="52" t="s">
+      <c r="B85" s="77" t="s">
         <v>81</v>
       </c>
-      <c r="C85" s="52"/>
-      <c r="D85" s="52"/>
-      <c r="E85" s="52"/>
-      <c r="F85" s="52"/>
+      <c r="C85" s="77"/>
+      <c r="D85" s="77"/>
+      <c r="E85" s="77"/>
+      <c r="F85" s="77"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B86" s="52"/>
-      <c r="C86" s="52"/>
-      <c r="D86" s="52"/>
-      <c r="E86" s="52"/>
-      <c r="F86" s="52"/>
+      <c r="B86" s="77"/>
+      <c r="C86" s="77"/>
+      <c r="D86" s="77"/>
+      <c r="E86" s="77"/>
+      <c r="F86" s="77"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B87" s="52"/>
-      <c r="C87" s="52"/>
-      <c r="D87" s="52"/>
-      <c r="E87" s="52"/>
-      <c r="F87" s="52"/>
+      <c r="B87" s="77"/>
+      <c r="C87" s="77"/>
+      <c r="D87" s="77"/>
+      <c r="E87" s="77"/>
+      <c r="F87" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
     <mergeCell ref="E58:F58"/>
     <mergeCell ref="E59:F59"/>
     <mergeCell ref="B85:F87"/>
@@ -4013,41 +4036,11 @@
     <mergeCell ref="E49:F49"/>
     <mergeCell ref="E50:F50"/>
     <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="E73:F73"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
some prints for tests. As well the updated excel with the completed Sign-Message interpreted correctly
</commit_message>
<xml_diff>
--- a/New Terminals/Sign-on/Sign-On.xlsx
+++ b/New Terminals/Sign-on/Sign-On.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\105864\Documents\Millennium\New Terminals\Sign-on\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65C7EC8-7D6D-4CC6-B480-6FD4A9B083F6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4988D1AC-8970-4C86-81D6-113F7F735AE4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A59DBA4C-956A-4B57-A1C8-C87C01DAE8BE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="261">
   <si>
     <r>
       <t>Test</t>
@@ -693,24 +693,12 @@
     <t>010000000000</t>
   </si>
   <si>
-    <t>69-70</t>
-  </si>
-  <si>
-    <t>71-72</t>
-  </si>
-  <si>
     <t>73-74</t>
   </si>
   <si>
     <t>75-76</t>
   </si>
   <si>
-    <t>78-79</t>
-  </si>
-  <si>
-    <t>80-81</t>
-  </si>
-  <si>
     <t>82-83</t>
   </si>
   <si>
@@ -726,9 +714,6 @@
     <t>01 11</t>
   </si>
   <si>
-    <t>01</t>
-  </si>
-  <si>
     <t>Game Type*=10001         Game Index**=001</t>
   </si>
   <si>
@@ -741,8 +726,147 @@
     <t>Game Type=17        Game Index=1</t>
   </si>
   <si>
+    <t>Password de Administrador/Gerente</t>
+  </si>
+  <si>
+    <t>Type=0011               SubType=0000</t>
+  </si>
+  <si>
+    <t>Type=3             SubType=0</t>
+  </si>
+  <si>
+    <t>10 - Application Message</t>
+  </si>
+  <si>
+    <t>F7 B8 92 9F</t>
+  </si>
+  <si>
+    <t>Control=0010        Sequence=1010</t>
+  </si>
+  <si>
+    <t>16 FF</t>
+  </si>
+  <si>
+    <t>0001011011111111</t>
+  </si>
+  <si>
+    <t>5887</t>
+  </si>
+  <si>
+    <t>2E 6F 9E</t>
+  </si>
+  <si>
+    <t>3043230</t>
+  </si>
+  <si>
+    <t>EC DE</t>
+  </si>
+  <si>
+    <t>60638</t>
+  </si>
+  <si>
+    <t>6F 9E EC DE</t>
+  </si>
+  <si>
+    <t>2E</t>
+  </si>
+  <si>
+    <t>9E 6F 2E</t>
+  </si>
+  <si>
+    <t>9A</t>
+  </si>
+  <si>
+    <t>Game Type*=10011       Game Index**=010</t>
+  </si>
+  <si>
+    <t>Game Type*=19      Game Index**=2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            X9A = M1lhão</t>
+  </si>
+  <si>
+    <t>65-66</t>
+  </si>
+  <si>
+    <t>67-68</t>
+  </si>
+  <si>
+    <t>Game Type*=00010       Game Index**=001</t>
+  </si>
+  <si>
+    <t>Game Type*=2       Game Index**=1</t>
+  </si>
+  <si>
+    <t>70-71</t>
+  </si>
+  <si>
+    <t>72-73</t>
+  </si>
+  <si>
+    <t>00 06</t>
+  </si>
+  <si>
+    <t>05 F0</t>
+  </si>
+  <si>
+    <t>X11 = Totobola Normal</t>
+  </si>
+  <si>
+    <t>77-78</t>
+  </si>
+  <si>
+    <t>01 96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0C </t>
+  </si>
+  <si>
+    <t>Game Type*=00001       Game Index**=100</t>
+  </si>
+  <si>
+    <t>Game Type*=  1       Game Index**= 4</t>
+  </si>
+  <si>
+    <t>X0C = Totoloto Quarta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00 04 </t>
+  </si>
+  <si>
+    <t>01 F1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01 F1 </t>
+  </si>
+  <si>
+    <t>Game Type*=  00001                Game Index**= 011</t>
+  </si>
+  <si>
+    <t>Game Type*= 1     Game Index**= 3</t>
+  </si>
+  <si>
+    <t>X0B = Totoloto Sábado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0B </t>
+  </si>
+  <si>
+    <t>11 00 06 05 F0 01 96</t>
+  </si>
+  <si>
+    <t>0110 = X04+X02</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">            </t>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x0004 = Control Rev. Present -&gt; 2 (bytes to follow)</t>
     </r>
     <r>
       <rPr>
@@ -752,18 +876,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>X89 = Euromilhões</t>
+      <t xml:space="preserve">                                                                  x0002 = Text Rev. Present -&gt; 2 (bytes to follow)</t>
     </r>
   </si>
   <si>
-    <t>Password de Administrador/Gerente</t>
+    <t>74-75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            X89 = Euromilhões</t>
+  </si>
+  <si>
+    <t>M1lhão</t>
+  </si>
+  <si>
+    <t>Games</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -818,8 +951,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -855,8 +995,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="36">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1303,11 +1449,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1382,9 +1543,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1469,7 +1627,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1494,9 +1651,6 @@
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1518,66 +1672,148 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1677,6 +1913,94 @@
         <a:xfrm>
           <a:off x="15450207" y="5485086"/>
           <a:ext cx="4953255" cy="4330923"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1168859</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>38322</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagem 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DB44B39-CEA6-4CEE-B7BB-32DAAEF0D3EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="607219" y="23229094"/>
+          <a:ext cx="8928559" cy="4324572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1097959</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>126359</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagem 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF3B6643-FA1F-4B75-B7F1-C3AADC9828B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12692063" y="28598813"/>
+          <a:ext cx="3937202" cy="2971953"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1985,10 +2309,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4A5A7B-0DA8-401C-B426-04429DCC05B9}">
-  <dimension ref="A2:S87"/>
+  <dimension ref="A2:S156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J56" sqref="J56"/>
+    <sheetView tabSelected="1" topLeftCell="G76" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="N85" sqref="N85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2008,25 +2332,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="112" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
     </row>
     <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="2:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="86" t="s">
+      <c r="B4" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="87"/>
+      <c r="C4" s="103"/>
       <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="88" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="89"/>
+      <c r="E4" s="104" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="105"/>
       <c r="G4" s="12" t="s">
         <v>24</v>
       </c>
@@ -2045,8 +2369,8 @@
         <v>4</v>
       </c>
       <c r="D5" s="5"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="91"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="107"/>
     </row>
     <row r="6" spans="2:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="6">
@@ -2116,10 +2440,10 @@
       <c r="D8" s="9">
         <v>2</v>
       </c>
-      <c r="E8" s="81" t="s">
+      <c r="E8" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="82"/>
+      <c r="F8" s="109"/>
       <c r="G8" s="12" t="s">
         <v>30</v>
       </c>
@@ -2143,10 +2467,10 @@
       <c r="D9" s="9">
         <v>1</v>
       </c>
-      <c r="E9" s="76" t="s">
+      <c r="E9" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="73"/>
+      <c r="F9" s="95"/>
       <c r="G9" s="16" t="s">
         <v>39</v>
       </c>
@@ -2168,10 +2492,10 @@
       <c r="D10" s="9">
         <v>4</v>
       </c>
-      <c r="E10" s="76" t="s">
+      <c r="E10" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="73"/>
+      <c r="F10" s="95"/>
       <c r="G10" s="19" t="s">
         <v>37</v>
       </c>
@@ -2195,10 +2519,10 @@
       <c r="D11" s="9">
         <v>2</v>
       </c>
-      <c r="E11" s="76" t="s">
+      <c r="E11" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="73"/>
+      <c r="F11" s="95"/>
       <c r="G11" s="20" t="s">
         <v>38</v>
       </c>
@@ -2222,10 +2546,10 @@
       <c r="D12" s="9">
         <v>2</v>
       </c>
-      <c r="E12" s="76" t="s">
+      <c r="E12" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="73"/>
+      <c r="F12" s="95"/>
       <c r="G12" s="19" t="s">
         <v>42</v>
       </c>
@@ -2249,10 +2573,10 @@
       <c r="D13" s="9">
         <v>8</v>
       </c>
-      <c r="E13" s="76" t="s">
+      <c r="E13" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="73"/>
+      <c r="F13" s="95"/>
       <c r="G13" s="20" t="s">
         <v>46</v>
       </c>
@@ -2276,10 +2600,10 @@
       <c r="D14" s="9">
         <v>8</v>
       </c>
-      <c r="E14" s="76" t="s">
+      <c r="E14" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="73"/>
+      <c r="F14" s="95"/>
       <c r="G14" s="16" t="s">
         <v>48</v>
       </c>
@@ -2301,10 +2625,10 @@
       <c r="D15" s="9">
         <v>8</v>
       </c>
-      <c r="E15" s="76" t="s">
+      <c r="E15" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="73"/>
+      <c r="F15" s="95"/>
       <c r="G15" s="19" t="s">
         <v>46</v>
       </c>
@@ -2328,10 +2652,10 @@
       <c r="D16" s="9">
         <v>8</v>
       </c>
-      <c r="E16" s="76" t="s">
+      <c r="E16" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="73"/>
+      <c r="F16" s="95"/>
       <c r="G16" s="19" t="s">
         <v>46</v>
       </c>
@@ -2355,10 +2679,10 @@
       <c r="D17" s="9">
         <v>8</v>
       </c>
-      <c r="E17" s="76" t="s">
+      <c r="E17" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="73"/>
+      <c r="F17" s="95"/>
       <c r="G17" s="19" t="s">
         <v>46</v>
       </c>
@@ -2382,10 +2706,10 @@
       <c r="D18" s="9">
         <v>8</v>
       </c>
-      <c r="E18" s="76" t="s">
+      <c r="E18" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="73"/>
+      <c r="F18" s="95"/>
       <c r="G18" s="19" t="s">
         <v>46</v>
       </c>
@@ -2409,10 +2733,10 @@
       <c r="D19" s="9">
         <v>4</v>
       </c>
-      <c r="E19" s="76" t="s">
+      <c r="E19" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="73"/>
+      <c r="F19" s="95"/>
       <c r="G19" s="19" t="s">
         <v>50</v>
       </c>
@@ -2436,10 +2760,10 @@
       <c r="D20" s="9">
         <v>4</v>
       </c>
-      <c r="E20" s="76" t="s">
+      <c r="E20" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="73"/>
+      <c r="F20" s="95"/>
       <c r="G20" s="16" t="s">
         <v>51</v>
       </c>
@@ -2463,10 +2787,10 @@
       <c r="D21" s="9">
         <v>4</v>
       </c>
-      <c r="E21" s="76" t="s">
+      <c r="E21" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="73"/>
+      <c r="F21" s="95"/>
       <c r="G21" s="16" t="s">
         <v>52</v>
       </c>
@@ -2490,10 +2814,10 @@
       <c r="D22" s="9">
         <v>4</v>
       </c>
-      <c r="E22" s="76" t="s">
+      <c r="E22" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="73"/>
+      <c r="F22" s="95"/>
       <c r="G22" s="16" t="s">
         <v>50</v>
       </c>
@@ -2517,10 +2841,10 @@
       <c r="D23" s="9">
         <v>4</v>
       </c>
-      <c r="E23" s="76" t="s">
+      <c r="E23" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="73"/>
+      <c r="F23" s="95"/>
       <c r="G23" s="24" t="s">
         <v>54</v>
       </c>
@@ -2544,10 +2868,10 @@
       <c r="D24" s="9">
         <v>4</v>
       </c>
-      <c r="E24" s="76" t="s">
+      <c r="E24" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="73"/>
+      <c r="F24" s="95"/>
       <c r="G24" s="19" t="s">
         <v>53</v>
       </c>
@@ -2571,10 +2895,10 @@
       <c r="D25" s="9">
         <v>4</v>
       </c>
-      <c r="E25" s="76" t="s">
+      <c r="E25" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="73"/>
+      <c r="F25" s="95"/>
       <c r="G25" s="19" t="s">
         <v>53</v>
       </c>
@@ -2598,10 +2922,10 @@
       <c r="D26" s="9">
         <v>4</v>
       </c>
-      <c r="E26" s="76" t="s">
+      <c r="E26" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="73"/>
+      <c r="F26" s="95"/>
       <c r="G26" s="19" t="s">
         <v>50</v>
       </c>
@@ -2625,10 +2949,10 @@
       <c r="D27" s="9">
         <v>4</v>
       </c>
-      <c r="E27" s="76" t="s">
+      <c r="E27" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="F27" s="73"/>
+      <c r="F27" s="95"/>
       <c r="G27" s="19" t="s">
         <v>50</v>
       </c>
@@ -2652,10 +2976,10 @@
       <c r="D28" s="9">
         <v>4</v>
       </c>
-      <c r="E28" s="76" t="s">
+      <c r="E28" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="F28" s="73"/>
+      <c r="F28" s="95"/>
       <c r="G28" s="19" t="s">
         <v>50</v>
       </c>
@@ -2679,10 +3003,10 @@
       <c r="D29" s="9">
         <v>4</v>
       </c>
-      <c r="E29" s="76" t="s">
+      <c r="E29" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="73"/>
+      <c r="F29" s="95"/>
       <c r="G29" s="19" t="s">
         <v>50</v>
       </c>
@@ -2706,10 +3030,10 @@
       <c r="D30" s="11">
         <v>4</v>
       </c>
-      <c r="E30" s="83" t="s">
+      <c r="E30" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="F30" s="75"/>
+      <c r="F30" s="111"/>
       <c r="G30" s="19" t="s">
         <v>50</v>
       </c>
@@ -2725,25 +3049,25 @@
     </row>
     <row r="31" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="34" spans="2:19" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B34" s="34" t="s">
+      <c r="B34" s="33" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="35" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="35"/>
+      <c r="B35" s="34"/>
     </row>
     <row r="36" spans="2:19" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="29"/>
+      <c r="C36" s="28"/>
       <c r="D36" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E36" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="F36" s="31"/>
+      <c r="E36" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" s="30"/>
       <c r="G36" s="12" t="s">
         <v>24</v>
       </c>
@@ -2762,8 +3086,8 @@
         <v>4</v>
       </c>
       <c r="D37" s="5"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="33"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="32"/>
       <c r="G37" s="16"/>
       <c r="H37" s="16"/>
       <c r="I37" s="16"/>
@@ -2836,10 +3160,10 @@
       <c r="D40" s="9">
         <v>2</v>
       </c>
-      <c r="E40" s="81" t="s">
+      <c r="E40" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="F40" s="82"/>
+      <c r="F40" s="109"/>
       <c r="G40" s="16" t="s">
         <v>82</v>
       </c>
@@ -2860,10 +3184,10 @@
       <c r="D41" s="9">
         <v>3</v>
       </c>
-      <c r="E41" s="76" t="s">
+      <c r="E41" s="101" t="s">
         <v>63</v>
       </c>
-      <c r="F41" s="73"/>
+      <c r="F41" s="95"/>
       <c r="G41" s="19" t="s">
         <v>85</v>
       </c>
@@ -2873,7 +3197,7 @@
       <c r="I41" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="J41" s="38" t="s">
+      <c r="J41" s="37" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2887,10 +3211,10 @@
       <c r="D42" s="9">
         <v>2</v>
       </c>
-      <c r="E42" s="76" t="s">
+      <c r="E42" s="101" t="s">
         <v>64</v>
       </c>
-      <c r="F42" s="73"/>
+      <c r="F42" s="95"/>
       <c r="G42" s="19" t="s">
         <v>89</v>
       </c>
@@ -2903,14 +3227,14 @@
       <c r="J42" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="L42" s="78"/>
-      <c r="M42" s="78"/>
-      <c r="N42" s="78"/>
-      <c r="O42" s="78"/>
-      <c r="P42" s="78"/>
-      <c r="Q42" s="78"/>
-      <c r="R42" s="78"/>
-      <c r="S42" s="78"/>
+      <c r="L42" s="115"/>
+      <c r="M42" s="115"/>
+      <c r="N42" s="115"/>
+      <c r="O42" s="115"/>
+      <c r="P42" s="115"/>
+      <c r="Q42" s="115"/>
+      <c r="R42" s="115"/>
+      <c r="S42" s="115"/>
     </row>
     <row r="43" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B43" s="8">
@@ -2922,10 +3246,10 @@
       <c r="D43" s="9">
         <v>2</v>
       </c>
-      <c r="E43" s="76" t="s">
+      <c r="E43" s="101" t="s">
         <v>65</v>
       </c>
-      <c r="F43" s="73"/>
+      <c r="F43" s="95"/>
       <c r="G43" s="16" t="s">
         <v>93</v>
       </c>
@@ -2949,20 +3273,20 @@
       <c r="D44" s="9">
         <v>1</v>
       </c>
-      <c r="E44" s="76" t="s">
+      <c r="E44" s="101" t="s">
         <v>66</v>
       </c>
-      <c r="F44" s="73"/>
-      <c r="G44" s="62" t="s">
+      <c r="F44" s="95"/>
+      <c r="G44" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="H44" s="62" t="s">
+      <c r="H44" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="I44" s="62" t="s">
+      <c r="I44" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="J44" s="63" t="s">
+      <c r="J44" s="61" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2976,10 +3300,10 @@
       <c r="D45" s="9">
         <v>2</v>
       </c>
-      <c r="E45" s="76" t="s">
+      <c r="E45" s="101" t="s">
         <v>67</v>
       </c>
-      <c r="F45" s="73"/>
+      <c r="F45" s="95"/>
       <c r="G45" s="12" t="s">
         <v>100</v>
       </c>
@@ -2989,7 +3313,7 @@
       <c r="I45" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="J45" s="39" t="s">
+      <c r="J45" s="38" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3003,10 +3327,10 @@
       <c r="D46" s="9">
         <v>1</v>
       </c>
-      <c r="E46" s="76" t="s">
+      <c r="E46" s="101" t="s">
         <v>68</v>
       </c>
-      <c r="F46" s="73"/>
+      <c r="F46" s="95"/>
       <c r="G46" s="19" t="s">
         <v>104</v>
       </c>
@@ -3016,7 +3340,7 @@
       <c r="I46" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="J46" s="38" t="s">
+      <c r="J46" s="37" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3030,10 +3354,10 @@
       <c r="D47" s="9">
         <v>4</v>
       </c>
-      <c r="E47" s="76" t="s">
+      <c r="E47" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="73"/>
+      <c r="F47" s="95"/>
       <c r="G47" s="18" t="s">
         <v>37</v>
       </c>
@@ -3057,26 +3381,26 @@
       <c r="D48" s="9">
         <v>1</v>
       </c>
-      <c r="E48" s="37" t="s">
+      <c r="E48" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="F48" s="37" t="s">
+      <c r="F48" s="36" t="s">
         <v>70</v>
       </c>
       <c r="G48" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="H48" s="40" t="s">
+      <c r="H48" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="I48" s="40" t="s">
+      <c r="I48" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="J48" s="41" t="s">
+      <c r="J48" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="K48" s="42"/>
-      <c r="L48" s="43" t="s">
+      <c r="K48" s="41"/>
+      <c r="L48" s="42" t="s">
         <v>114</v>
       </c>
     </row>
@@ -3090,10 +3414,10 @@
       <c r="D49" s="9">
         <v>2</v>
       </c>
-      <c r="E49" s="76" t="s">
+      <c r="E49" s="101" t="s">
         <v>71</v>
       </c>
-      <c r="F49" s="73"/>
+      <c r="F49" s="95"/>
       <c r="G49" s="19" t="s">
         <v>116</v>
       </c>
@@ -3103,7 +3427,7 @@
       <c r="I49" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="J49" s="44" t="s">
+      <c r="J49" s="43" t="s">
         <v>119</v>
       </c>
     </row>
@@ -3117,10 +3441,10 @@
       <c r="D50" s="9">
         <v>2</v>
       </c>
-      <c r="E50" s="76" t="s">
+      <c r="E50" s="101" t="s">
         <v>72</v>
       </c>
-      <c r="F50" s="73"/>
+      <c r="F50" s="95"/>
       <c r="G50" s="16" t="s">
         <v>120</v>
       </c>
@@ -3141,10 +3465,10 @@
       <c r="D51" s="9">
         <v>2</v>
       </c>
-      <c r="E51" s="76" t="s">
+      <c r="E51" s="101" t="s">
         <v>73</v>
       </c>
-      <c r="F51" s="73"/>
+      <c r="F51" s="95"/>
       <c r="G51" s="16" t="s">
         <v>120</v>
       </c>
@@ -3165,10 +3489,10 @@
       <c r="D52" s="9">
         <v>2</v>
       </c>
-      <c r="E52" s="76" t="s">
+      <c r="E52" s="101" t="s">
         <v>74</v>
       </c>
-      <c r="F52" s="73"/>
+      <c r="F52" s="95"/>
       <c r="G52" s="16" t="s">
         <v>38</v>
       </c>
@@ -3192,10 +3516,10 @@
       <c r="D53" s="9">
         <v>4</v>
       </c>
-      <c r="E53" s="76" t="s">
+      <c r="E53" s="101" t="s">
         <v>75</v>
       </c>
-      <c r="F53" s="73"/>
+      <c r="F53" s="95"/>
       <c r="G53" s="19" t="s">
         <v>50</v>
       </c>
@@ -3219,10 +3543,10 @@
       <c r="D54" s="9">
         <v>4</v>
       </c>
-      <c r="E54" s="76" t="s">
+      <c r="E54" s="101" t="s">
         <v>76</v>
       </c>
-      <c r="F54" s="73"/>
+      <c r="F54" s="95"/>
       <c r="G54" s="18" t="s">
         <v>121</v>
       </c>
@@ -3246,10 +3570,10 @@
       <c r="D55" s="9">
         <v>2</v>
       </c>
-      <c r="E55" s="76" t="s">
+      <c r="E55" s="101" t="s">
         <v>77</v>
       </c>
-      <c r="F55" s="73"/>
+      <c r="F55" s="95"/>
       <c r="G55" s="18" t="s">
         <v>122</v>
       </c>
@@ -3260,7 +3584,7 @@
         <v>123</v>
       </c>
       <c r="J55" s="18" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="56" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3273,10 +3597,10 @@
       <c r="D56" s="9">
         <v>2</v>
       </c>
-      <c r="E56" s="76" t="s">
+      <c r="E56" s="101" t="s">
         <v>78</v>
       </c>
-      <c r="F56" s="73"/>
+      <c r="F56" s="95"/>
       <c r="G56" s="19" t="s">
         <v>38</v>
       </c>
@@ -3286,7 +3610,7 @@
       <c r="I56" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="J56" s="38" t="s">
+      <c r="J56" s="37" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3300,10 +3624,10 @@
       <c r="D57" s="9">
         <v>8</v>
       </c>
-      <c r="E57" s="76" t="s">
+      <c r="E57" s="101" t="s">
         <v>78</v>
       </c>
-      <c r="F57" s="73"/>
+      <c r="F57" s="95"/>
       <c r="G57" s="19" t="s">
         <v>46</v>
       </c>
@@ -3313,7 +3637,7 @@
       <c r="I57" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="J57" s="38" t="s">
+      <c r="J57" s="37" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3327,10 +3651,10 @@
       <c r="D58" s="9">
         <v>4</v>
       </c>
-      <c r="E58" s="76" t="s">
+      <c r="E58" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="F58" s="73"/>
+      <c r="F58" s="95"/>
       <c r="G58" s="18" t="s">
         <v>125</v>
       </c>
@@ -3354,10 +3678,10 @@
       <c r="D59" s="9">
         <v>4</v>
       </c>
-      <c r="E59" s="76" t="s">
+      <c r="E59" s="101" t="s">
         <v>80</v>
       </c>
-      <c r="F59" s="73"/>
+      <c r="F59" s="95"/>
       <c r="G59" s="18" t="s">
         <v>130</v>
       </c>
@@ -3373,110 +3697,110 @@
     </row>
     <row r="60" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="61" spans="1:16" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B61" s="79" t="s">
+      <c r="B61" s="116" t="s">
         <v>151</v>
       </c>
-      <c r="C61" s="79"/>
-      <c r="D61" s="79"/>
-      <c r="E61" s="79"/>
-      <c r="F61" s="79"/>
-      <c r="L61" s="56" t="s">
+      <c r="C61" s="116"/>
+      <c r="D61" s="116"/>
+      <c r="E61" s="116"/>
+      <c r="F61" s="116"/>
+      <c r="L61" s="54" t="s">
         <v>167</v>
       </c>
-      <c r="M61" s="57" t="s">
+      <c r="M61" s="55" t="s">
         <v>168</v>
       </c>
-      <c r="N61" s="57" t="s">
+      <c r="N61" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="O61" s="57" t="s">
+      <c r="O61" s="55" t="s">
         <v>170</v>
       </c>
-      <c r="P61" s="58" t="s">
+      <c r="P61" s="56" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="62" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B62" s="45">
+      <c r="B62" s="44">
         <v>57</v>
       </c>
-      <c r="C62" s="46">
+      <c r="C62" s="45">
         <v>57</v>
       </c>
-      <c r="D62" s="46">
+      <c r="D62" s="45">
         <v>1</v>
       </c>
-      <c r="E62" s="51" t="s">
+      <c r="E62" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="F62" s="52"/>
-      <c r="G62" s="54" t="s">
+      <c r="F62" s="51"/>
+      <c r="G62" s="93" t="s">
         <v>157</v>
       </c>
-      <c r="H62" s="16" t="s">
+      <c r="H62" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="I62" s="16" t="s">
+      <c r="I62" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="J62" s="12" t="s">
+      <c r="J62" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="L62" s="68">
+      <c r="L62" s="65">
         <v>1</v>
       </c>
-      <c r="M62" s="69" t="s">
+      <c r="M62" s="66" t="s">
         <v>172</v>
       </c>
-      <c r="N62" s="70">
+      <c r="N62" s="67">
         <v>17</v>
       </c>
-      <c r="O62" s="70">
+      <c r="O62" s="67">
         <v>1</v>
       </c>
-      <c r="P62" s="71" t="s">
+      <c r="P62" s="68" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="63" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B63" s="47">
+      <c r="B63" s="46">
         <v>58</v>
       </c>
-      <c r="C63" s="48">
+      <c r="C63" s="47">
         <v>58</v>
       </c>
-      <c r="D63" s="48">
+      <c r="D63" s="47">
         <v>1</v>
       </c>
-      <c r="E63" s="53" t="s">
+      <c r="E63" s="52" t="s">
         <v>134</v>
       </c>
-      <c r="F63" s="27"/>
-      <c r="G63" s="16" t="s">
+      <c r="F63" s="26"/>
+      <c r="G63" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="H63" s="16" t="s">
+      <c r="H63" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="I63" s="16" t="s">
+      <c r="I63" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="J63" s="12" t="s">
+      <c r="J63" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="L63" s="49">
-        <v>2</v>
-      </c>
-      <c r="M63" s="59" t="s">
+      <c r="L63" s="48">
+        <v>2</v>
+      </c>
+      <c r="M63" s="57" t="s">
         <v>174</v>
       </c>
-      <c r="N63" s="50">
+      <c r="N63" s="49">
         <v>19</v>
       </c>
-      <c r="O63" s="50">
-        <v>2</v>
-      </c>
-      <c r="P63" s="37" t="s">
+      <c r="O63" s="49">
+        <v>2</v>
+      </c>
+      <c r="P63" s="36" t="s">
         <v>175</v>
       </c>
     </row>
@@ -3484,46 +3808,46 @@
       <c r="A64" s="12">
         <v>59</v>
       </c>
-      <c r="B64" s="49" t="s">
+      <c r="B64" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="C64" s="50" t="s">
+      <c r="C64" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="D64" s="50">
+      <c r="D64" s="49">
         <v>1</v>
       </c>
-      <c r="E64" s="50" t="s">
+      <c r="E64" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="F64" s="37" t="s">
+      <c r="F64" s="36" t="s">
         <v>138</v>
       </c>
       <c r="G64" s="19" t="s">
         <v>161</v>
       </c>
       <c r="H64" s="25" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="I64" s="25" t="s">
-        <v>216</v>
-      </c>
-      <c r="J64" s="67" t="s">
-        <v>217</v>
-      </c>
-      <c r="L64" s="49">
+        <v>211</v>
+      </c>
+      <c r="J64" s="64" t="s">
+        <v>258</v>
+      </c>
+      <c r="L64" s="48">
         <v>3</v>
       </c>
-      <c r="M64" s="59" t="s">
+      <c r="M64" s="57" t="s">
         <v>176</v>
       </c>
-      <c r="N64" s="50">
-        <v>2</v>
-      </c>
-      <c r="O64" s="50">
+      <c r="N64" s="49">
+        <v>2</v>
+      </c>
+      <c r="O64" s="49">
         <v>1</v>
       </c>
-      <c r="P64" s="37" t="s">
+      <c r="P64" s="36" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3531,44 +3855,44 @@
       <c r="A65" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="B65" s="49" t="s">
+      <c r="B65" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="C65" s="50" t="s">
+      <c r="C65" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="D65" s="50">
-        <v>2</v>
-      </c>
-      <c r="E65" s="72" t="s">
+      <c r="D65" s="49">
+        <v>2</v>
+      </c>
+      <c r="E65" s="94" t="s">
         <v>141</v>
       </c>
-      <c r="F65" s="73"/>
-      <c r="G65" s="16" t="s">
+      <c r="F65" s="95"/>
+      <c r="G65" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="H65" s="16" t="s">
+      <c r="H65" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="I65" s="16" t="s">
+      <c r="I65" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="J65" s="36" t="s">
+      <c r="J65" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="L65" s="49">
+      <c r="L65" s="48">
         <v>4</v>
       </c>
-      <c r="M65" s="59" t="s">
+      <c r="M65" s="57" t="s">
         <v>178</v>
       </c>
-      <c r="N65" s="50">
+      <c r="N65" s="49">
         <v>4</v>
       </c>
-      <c r="O65" s="50">
+      <c r="O65" s="49">
         <v>1</v>
       </c>
-      <c r="P65" s="37" t="s">
+      <c r="P65" s="36" t="s">
         <v>179</v>
       </c>
     </row>
@@ -3576,19 +3900,19 @@
       <c r="A66" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="B66" s="49" t="s">
+      <c r="B66" s="48" t="s">
         <v>142</v>
       </c>
-      <c r="C66" s="50" t="s">
+      <c r="C66" s="49" t="s">
         <v>143</v>
       </c>
-      <c r="D66" s="50">
-        <v>2</v>
-      </c>
-      <c r="E66" s="72" t="s">
+      <c r="D66" s="49">
+        <v>2</v>
+      </c>
+      <c r="E66" s="94" t="s">
         <v>144</v>
       </c>
-      <c r="F66" s="73"/>
+      <c r="F66" s="95"/>
       <c r="G66" s="16" t="s">
         <v>120</v>
       </c>
@@ -3601,107 +3925,107 @@
       <c r="J66" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="L66" s="49">
+      <c r="L66" s="48">
         <v>5</v>
       </c>
-      <c r="M66" s="59" t="s">
+      <c r="M66" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="N66" s="50">
+      <c r="N66" s="49">
         <v>1</v>
       </c>
-      <c r="O66" s="50">
+      <c r="O66" s="49">
         <v>3</v>
       </c>
-      <c r="P66" s="37" t="s">
+      <c r="P66" s="36" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="12" t="s">
+    <row r="67" spans="1:16" s="82" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="63" t="s">
         <v>192</v>
       </c>
-      <c r="B67" s="49" t="s">
+      <c r="B67" s="73" t="s">
         <v>145</v>
       </c>
-      <c r="C67" s="50" t="s">
+      <c r="C67" s="74" t="s">
         <v>146</v>
       </c>
-      <c r="D67" s="50">
-        <v>2</v>
-      </c>
-      <c r="E67" s="72" t="s">
+      <c r="D67" s="74">
+        <v>2</v>
+      </c>
+      <c r="E67" s="96" t="s">
         <v>147</v>
       </c>
-      <c r="F67" s="73"/>
-      <c r="G67" s="16" t="s">
+      <c r="F67" s="97"/>
+      <c r="G67" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="H67" s="16" t="s">
+      <c r="H67" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="I67" s="16" t="s">
+      <c r="I67" s="24" t="s">
         <v>196</v>
       </c>
-      <c r="J67" s="12" t="s">
+      <c r="J67" s="63" t="s">
         <v>194</v>
       </c>
-      <c r="L67" s="49">
+      <c r="L67" s="80">
         <v>6</v>
       </c>
-      <c r="M67" s="59" t="s">
+      <c r="M67" s="83" t="s">
         <v>182</v>
       </c>
-      <c r="N67" s="50">
+      <c r="N67" s="81">
         <v>1</v>
       </c>
-      <c r="O67" s="50">
+      <c r="O67" s="81">
         <v>4</v>
       </c>
-      <c r="P67" s="37" t="s">
+      <c r="P67" s="84" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="12" t="s">
+    <row r="68" spans="1:16" s="82" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="63" t="s">
         <v>193</v>
       </c>
-      <c r="B68" s="47" t="s">
+      <c r="B68" s="75" t="s">
         <v>148</v>
       </c>
-      <c r="C68" s="48" t="s">
+      <c r="C68" s="76" t="s">
         <v>149</v>
       </c>
-      <c r="D68" s="48">
-        <v>2</v>
-      </c>
-      <c r="E68" s="74" t="s">
+      <c r="D68" s="76">
+        <v>2</v>
+      </c>
+      <c r="E68" s="98" t="s">
         <v>150</v>
       </c>
-      <c r="F68" s="75"/>
-      <c r="G68" s="12" t="s">
+      <c r="F68" s="99"/>
+      <c r="G68" s="63" t="s">
         <v>198</v>
       </c>
-      <c r="H68" s="16" t="s">
+      <c r="H68" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="I68" s="16" t="s">
+      <c r="I68" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="J68" s="12"/>
-      <c r="L68" s="49">
+      <c r="J68" s="63"/>
+      <c r="L68" s="80">
         <v>7</v>
       </c>
-      <c r="M68" s="59" t="s">
+      <c r="M68" s="83" t="s">
         <v>184</v>
       </c>
-      <c r="N68" s="50">
+      <c r="N68" s="81">
         <v>16</v>
       </c>
-      <c r="O68" s="50">
+      <c r="O68" s="81">
         <v>1</v>
       </c>
-      <c r="P68" s="37" t="s">
+      <c r="P68" s="84" t="s">
         <v>185</v>
       </c>
     </row>
@@ -3709,320 +4033,1146 @@
       <c r="H69" s="12"/>
       <c r="I69" s="12"/>
       <c r="J69" s="12"/>
-      <c r="L69" s="49">
+      <c r="L69" s="48">
         <v>8</v>
       </c>
-      <c r="M69" s="59" t="s">
+      <c r="M69" s="57" t="s">
         <v>186</v>
       </c>
-      <c r="N69" s="50">
+      <c r="N69" s="49">
         <v>16</v>
       </c>
-      <c r="O69" s="50">
-        <v>2</v>
-      </c>
-      <c r="P69" s="37" t="s">
+      <c r="O69" s="49">
+        <v>2</v>
+      </c>
+      <c r="P69" s="36" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:16" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="65" t="s">
+      <c r="A70" s="62" t="s">
+        <v>206</v>
+      </c>
+      <c r="B70" s="63" t="s">
+        <v>205</v>
+      </c>
+      <c r="G70" s="63" t="s">
+        <v>207</v>
+      </c>
+      <c r="L70" s="46">
+        <v>9</v>
+      </c>
+      <c r="M70" s="58" t="s">
+        <v>188</v>
+      </c>
+      <c r="N70" s="47">
+        <v>2</v>
+      </c>
+      <c r="O70" s="47">
+        <v>3</v>
+      </c>
+      <c r="P70" s="59" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="72" spans="1:16" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="18">
+        <v>64</v>
+      </c>
+      <c r="B72" s="65" t="s">
+        <v>135</v>
+      </c>
+      <c r="C72" s="67" t="s">
+        <v>136</v>
+      </c>
+      <c r="D72" s="67">
+        <v>1</v>
+      </c>
+      <c r="E72" s="67" t="s">
+        <v>137</v>
+      </c>
+      <c r="F72" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="G72" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="H72" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="I72" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="J72" s="64" t="s">
+        <v>231</v>
+      </c>
+      <c r="L72" s="117" t="s">
+        <v>209</v>
+      </c>
+      <c r="M72" s="117"/>
+      <c r="N72" s="117"/>
+    </row>
+    <row r="73" spans="1:16" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A73" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="B73" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="C73" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="D73" s="49">
+        <v>2</v>
+      </c>
+      <c r="E73" s="94" t="s">
+        <v>141</v>
+      </c>
+      <c r="F73" s="95"/>
+      <c r="G73" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="H73" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="I73" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="J73" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="L73" s="117" t="s">
         <v>210</v>
       </c>
-      <c r="B70" s="66" t="s">
-        <v>209</v>
-      </c>
-      <c r="G70" s="66" t="s">
-        <v>211</v>
-      </c>
-      <c r="L70" s="47">
-        <v>9</v>
-      </c>
-      <c r="M70" s="60" t="s">
-        <v>188</v>
-      </c>
-      <c r="N70" s="48">
-        <v>2</v>
-      </c>
-      <c r="O70" s="48">
-        <v>3</v>
-      </c>
-      <c r="P70" s="61" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="72" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="12">
-        <v>68</v>
-      </c>
-      <c r="B72" s="49" t="s">
-        <v>135</v>
-      </c>
-      <c r="C72" s="50" t="s">
-        <v>136</v>
-      </c>
-      <c r="D72" s="50">
-        <v>1</v>
-      </c>
-      <c r="E72" s="50" t="s">
-        <v>137</v>
-      </c>
-      <c r="F72" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="G72" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="H72" s="12">
-        <v>1</v>
-      </c>
-      <c r="I72" s="12">
-        <v>1</v>
-      </c>
-      <c r="L72" s="80" t="s">
-        <v>214</v>
-      </c>
-      <c r="M72" s="80"/>
-      <c r="N72" s="80"/>
-    </row>
-    <row r="73" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="B73" s="49" t="s">
-        <v>139</v>
-      </c>
-      <c r="C73" s="50" t="s">
-        <v>140</v>
-      </c>
-      <c r="D73" s="50">
-        <v>2</v>
-      </c>
-      <c r="E73" s="72" t="s">
-        <v>141</v>
-      </c>
-      <c r="F73" s="73"/>
-      <c r="G73" s="55"/>
-      <c r="L73" s="80" t="s">
-        <v>215</v>
-      </c>
-      <c r="M73" s="80"/>
+      <c r="M73" s="117"/>
     </row>
     <row r="74" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="B74" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="C74" s="49" t="s">
+        <v>143</v>
+      </c>
+      <c r="D74" s="49">
+        <v>2</v>
+      </c>
+      <c r="E74" s="94" t="s">
+        <v>144</v>
+      </c>
+      <c r="F74" s="95"/>
+      <c r="G74" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="H74" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="I74" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="J74" s="71" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A75" s="77" t="s">
+        <v>201</v>
+      </c>
+      <c r="B75" s="73" t="s">
+        <v>145</v>
+      </c>
+      <c r="C75" s="74" t="s">
+        <v>146</v>
+      </c>
+      <c r="D75" s="74">
+        <v>2</v>
+      </c>
+      <c r="E75" s="96" t="s">
+        <v>147</v>
+      </c>
+      <c r="F75" s="97"/>
+      <c r="G75" s="78"/>
+      <c r="H75" s="77"/>
+      <c r="I75" s="77"/>
+      <c r="J75" s="79"/>
+      <c r="K75" s="79"/>
+    </row>
+    <row r="76" spans="1:16" ht="26.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A76" s="77" t="s">
         <v>202</v>
       </c>
-      <c r="B74" s="49" t="s">
+      <c r="B76" s="75" t="s">
+        <v>148</v>
+      </c>
+      <c r="C76" s="76" t="s">
+        <v>149</v>
+      </c>
+      <c r="D76" s="76">
+        <v>2</v>
+      </c>
+      <c r="E76" s="98" t="s">
+        <v>150</v>
+      </c>
+      <c r="F76" s="99"/>
+      <c r="G76" s="78"/>
+      <c r="H76" s="77"/>
+      <c r="I76" s="77"/>
+      <c r="J76" s="79"/>
+      <c r="K76" s="79"/>
+    </row>
+    <row r="77" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="G77" s="89" t="s">
+        <v>254</v>
+      </c>
+      <c r="H77" s="71"/>
+      <c r="I77" s="71"/>
+    </row>
+    <row r="78" spans="1:16" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="18">
+        <v>69</v>
+      </c>
+      <c r="B78" s="65" t="s">
+        <v>135</v>
+      </c>
+      <c r="C78" s="67" t="s">
+        <v>136</v>
+      </c>
+      <c r="D78" s="67">
+        <v>1</v>
+      </c>
+      <c r="E78" s="67" t="s">
+        <v>137</v>
+      </c>
+      <c r="F78" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="G78" s="19">
+        <v>11</v>
+      </c>
+      <c r="H78" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="I78" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="J78" s="18" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="B79" s="65" t="s">
+        <v>139</v>
+      </c>
+      <c r="C79" s="67" t="s">
+        <v>140</v>
+      </c>
+      <c r="D79" s="67">
+        <v>2</v>
+      </c>
+      <c r="E79" s="90" t="s">
+        <v>141</v>
+      </c>
+      <c r="F79" s="91"/>
+      <c r="G79" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="H79" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="I79" s="19"/>
+      <c r="J79" s="100" t="s">
+        <v>256</v>
+      </c>
+      <c r="K79" s="100"/>
+      <c r="L79" s="100"/>
+      <c r="M79" s="100"/>
+    </row>
+    <row r="80" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="B80" s="65" t="s">
         <v>142</v>
       </c>
-      <c r="C74" s="50" t="s">
+      <c r="C80" s="67" t="s">
         <v>143</v>
       </c>
-      <c r="D74" s="50">
-        <v>2</v>
-      </c>
-      <c r="E74" s="64" t="s">
+      <c r="D80" s="67">
+        <v>2</v>
+      </c>
+      <c r="E80" s="90" t="s">
         <v>144</v>
       </c>
-      <c r="F74" s="26"/>
-      <c r="G74" s="55"/>
-    </row>
-    <row r="75" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="12" t="s">
+      <c r="F80" s="91"/>
+      <c r="G80" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="H80" s="19"/>
+      <c r="I80" s="19"/>
+      <c r="J80" s="92"/>
+      <c r="K80" s="92"/>
+      <c r="L80" s="92"/>
+      <c r="M80" s="92"/>
+    </row>
+    <row r="81" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A81" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="B81" s="65" t="s">
+        <v>145</v>
+      </c>
+      <c r="C81" s="67" t="s">
+        <v>146</v>
+      </c>
+      <c r="D81" s="67">
+        <v>2</v>
+      </c>
+      <c r="E81" s="90" t="s">
+        <v>147</v>
+      </c>
+      <c r="F81" s="91"/>
+      <c r="G81" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="H81" s="19"/>
+      <c r="I81" s="19"/>
+      <c r="J81" s="92"/>
+    </row>
+    <row r="82" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="63" t="s">
+        <v>204</v>
+      </c>
+      <c r="B82" s="75" t="s">
+        <v>148</v>
+      </c>
+      <c r="C82" s="76" t="s">
+        <v>149</v>
+      </c>
+      <c r="D82" s="76">
+        <v>2</v>
+      </c>
+      <c r="E82" s="87" t="s">
+        <v>150</v>
+      </c>
+      <c r="F82" s="88"/>
+      <c r="G82" s="24"/>
+      <c r="H82" s="24"/>
+      <c r="I82" s="24"/>
+      <c r="J82" s="41"/>
+    </row>
+    <row r="83" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="L83" s="118" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="18">
+        <v>74</v>
+      </c>
+      <c r="B84" s="65" t="s">
+        <v>135</v>
+      </c>
+      <c r="C84" s="67" t="s">
+        <v>136</v>
+      </c>
+      <c r="D84" s="67">
+        <v>1</v>
+      </c>
+      <c r="E84" s="67" t="s">
+        <v>137</v>
+      </c>
+      <c r="F84" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="G84" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="H84" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="I84" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="J84" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="L84" s="118" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A85" s="71" t="s">
+        <v>202</v>
+      </c>
+      <c r="B85" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="C85" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="D85" s="49">
+        <v>2</v>
+      </c>
+      <c r="E85" s="72" t="s">
+        <v>141</v>
+      </c>
+      <c r="F85" s="70"/>
+      <c r="G85" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="H85" s="16"/>
+      <c r="I85" s="16"/>
+      <c r="J85" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="L85" s="118" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A86" s="71" t="s">
+        <v>241</v>
+      </c>
+      <c r="B86" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="C86" s="49" t="s">
+        <v>143</v>
+      </c>
+      <c r="D86" s="49">
+        <v>2</v>
+      </c>
+      <c r="E86" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="F86" s="70"/>
+      <c r="G86" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="H86" s="16"/>
+      <c r="I86" s="16"/>
+      <c r="L86" s="118" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A87" s="63" t="s">
         <v>203</v>
       </c>
-      <c r="B75" s="49" t="s">
+      <c r="B87" s="73" t="s">
         <v>145</v>
       </c>
-      <c r="C75" s="50" t="s">
+      <c r="C87" s="74" t="s">
         <v>146</v>
       </c>
-      <c r="D75" s="50">
-        <v>2</v>
-      </c>
-      <c r="E75" s="64" t="s">
+      <c r="D87" s="74">
+        <v>2</v>
+      </c>
+      <c r="E87" s="85" t="s">
         <v>147</v>
       </c>
-      <c r="F75" s="26"/>
-      <c r="G75" s="55"/>
-    </row>
-    <row r="76" spans="1:16" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="12" t="s">
+      <c r="F87" s="86"/>
+      <c r="G87" s="24"/>
+      <c r="H87" s="24"/>
+      <c r="I87" s="24"/>
+      <c r="J87" s="41"/>
+      <c r="L87" s="118" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="63" t="s">
         <v>204</v>
       </c>
-      <c r="B76" s="47" t="s">
+      <c r="B88" s="75" t="s">
         <v>148</v>
       </c>
-      <c r="C76" s="48" t="s">
+      <c r="C88" s="76" t="s">
         <v>149</v>
       </c>
-      <c r="D76" s="48">
-        <v>2</v>
-      </c>
-      <c r="E76" s="53" t="s">
+      <c r="D88" s="76">
+        <v>2</v>
+      </c>
+      <c r="E88" s="87" t="s">
         <v>150</v>
       </c>
-      <c r="F76" s="27"/>
-      <c r="G76" s="55"/>
-    </row>
-    <row r="77" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="78" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="12">
+      <c r="F88" s="88"/>
+      <c r="G88" s="24"/>
+      <c r="H88" s="24"/>
+      <c r="I88" s="24"/>
+      <c r="J88" s="41"/>
+      <c r="L88" s="118" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="90" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="18">
+        <v>79</v>
+      </c>
+      <c r="B90" s="65" t="s">
+        <v>135</v>
+      </c>
+      <c r="C90" s="67" t="s">
+        <v>136</v>
+      </c>
+      <c r="D90" s="67">
+        <v>1</v>
+      </c>
+      <c r="E90" s="67" t="s">
+        <v>137</v>
+      </c>
+      <c r="F90" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="G90" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="H90" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="I90" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="J90" s="18" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A91" s="71" t="s">
+        <v>202</v>
+      </c>
+      <c r="B91" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="C91" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="D91" s="49">
+        <v>2</v>
+      </c>
+      <c r="E91" s="72" t="s">
+        <v>141</v>
+      </c>
+      <c r="F91" s="70"/>
+      <c r="G91" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="H91" s="16"/>
+      <c r="I91" s="16"/>
+      <c r="J91" s="35" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A92" s="71" t="s">
+        <v>241</v>
+      </c>
+      <c r="B92" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="C92" s="49" t="s">
+        <v>143</v>
+      </c>
+      <c r="D92" s="49">
+        <v>2</v>
+      </c>
+      <c r="E92" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="F92" s="70"/>
+      <c r="G92" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="H92" s="16"/>
+      <c r="I92" s="16"/>
+    </row>
+    <row r="93" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A93" s="63" t="s">
+        <v>203</v>
+      </c>
+      <c r="B93" s="73" t="s">
+        <v>145</v>
+      </c>
+      <c r="C93" s="74" t="s">
+        <v>146</v>
+      </c>
+      <c r="D93" s="74">
+        <v>2</v>
+      </c>
+      <c r="E93" s="85" t="s">
+        <v>147</v>
+      </c>
+      <c r="F93" s="86"/>
+      <c r="G93" s="24"/>
+      <c r="H93" s="24"/>
+      <c r="I93" s="24"/>
+      <c r="J93" s="41"/>
+    </row>
+    <row r="94" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A94" s="63" t="s">
+        <v>204</v>
+      </c>
+      <c r="B94" s="75" t="s">
+        <v>148</v>
+      </c>
+      <c r="C94" s="76" t="s">
+        <v>149</v>
+      </c>
+      <c r="D94" s="76">
+        <v>2</v>
+      </c>
+      <c r="E94" s="87" t="s">
+        <v>150</v>
+      </c>
+      <c r="F94" s="88"/>
+      <c r="G94" s="24"/>
+      <c r="H94" s="24"/>
+      <c r="I94" s="24"/>
+      <c r="J94" s="41"/>
+    </row>
+    <row r="95" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B99" s="114" t="s">
+        <v>81</v>
+      </c>
+      <c r="C99" s="114"/>
+      <c r="D99" s="114"/>
+      <c r="E99" s="114"/>
+      <c r="F99" s="114"/>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B100" s="114"/>
+      <c r="C100" s="114"/>
+      <c r="D100" s="114"/>
+      <c r="E100" s="114"/>
+      <c r="F100" s="114"/>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B101" s="114"/>
+      <c r="C101" s="114"/>
+      <c r="D101" s="114"/>
+      <c r="E101" s="114"/>
+      <c r="F101" s="114"/>
+    </row>
+    <row r="128" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C128" t="s">
+        <v>225</v>
+      </c>
+      <c r="D128" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="129" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="E129" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="132" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="133" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B133" s="102" t="s">
+        <v>0</v>
+      </c>
+      <c r="C133" s="103"/>
+      <c r="D133" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E133" s="104" t="s">
+        <v>2</v>
+      </c>
+      <c r="F133" s="105"/>
+      <c r="G133" s="69" t="s">
+        <v>24</v>
+      </c>
+      <c r="H133" s="69" t="s">
+        <v>27</v>
+      </c>
+      <c r="I133" s="69" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="134" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B134" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D134" s="5"/>
+      <c r="E134" s="106"/>
+      <c r="F134" s="107"/>
+      <c r="G134" s="16"/>
+      <c r="H134" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="I134" s="16"/>
+    </row>
+    <row r="135" spans="2:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B135" s="6">
+        <v>1</v>
+      </c>
+      <c r="C135" s="4">
+        <v>1</v>
+      </c>
+      <c r="D135" s="4">
+        <v>1</v>
+      </c>
+      <c r="E135" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F135" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G135" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="H135" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="I135" s="16"/>
+    </row>
+    <row r="136" spans="2:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B136" s="6">
+        <v>2</v>
+      </c>
+      <c r="C136" s="4">
+        <v>2</v>
+      </c>
+      <c r="D136" s="4">
+        <v>1</v>
+      </c>
+      <c r="E136" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F136" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G136" s="53">
+        <v>30</v>
+      </c>
+      <c r="H136" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="I136" s="17" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="137" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B137" s="8">
+        <v>3</v>
+      </c>
+      <c r="C137" s="9">
+        <v>4</v>
+      </c>
+      <c r="D137" s="9">
+        <v>2</v>
+      </c>
+      <c r="E137" s="108" t="s">
+        <v>9</v>
+      </c>
+      <c r="F137" s="109"/>
+      <c r="G137" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="H137" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="I137" s="16" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="138" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B138" s="8">
+        <v>5</v>
+      </c>
+      <c r="C138" s="9">
+        <v>7</v>
+      </c>
+      <c r="D138" s="9">
+        <v>3</v>
+      </c>
+      <c r="E138" s="101" t="s">
+        <v>63</v>
+      </c>
+      <c r="F138" s="95"/>
+      <c r="G138" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="H138" s="16"/>
+      <c r="I138" s="16" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="139" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B139" s="8">
+        <v>8</v>
+      </c>
+      <c r="C139" s="9">
+        <v>9</v>
+      </c>
+      <c r="D139" s="9">
+        <v>2</v>
+      </c>
+      <c r="E139" s="101" t="s">
+        <v>64</v>
+      </c>
+      <c r="F139" s="95"/>
+      <c r="G139" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="H139" s="16"/>
+      <c r="I139" s="16" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="140" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B140" s="8">
+        <v>10</v>
+      </c>
+      <c r="C140" s="9">
+        <v>11</v>
+      </c>
+      <c r="D140" s="9">
+        <v>2</v>
+      </c>
+      <c r="E140" s="101" t="s">
+        <v>65</v>
+      </c>
+      <c r="F140" s="95"/>
+      <c r="G140" s="16"/>
+      <c r="H140" s="16"/>
+      <c r="I140" s="16"/>
+    </row>
+    <row r="141" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B141" s="8">
+        <v>12</v>
+      </c>
+      <c r="C141" s="9">
+        <v>12</v>
+      </c>
+      <c r="D141" s="9">
+        <v>1</v>
+      </c>
+      <c r="E141" s="101" t="s">
+        <v>66</v>
+      </c>
+      <c r="F141" s="95"/>
+      <c r="G141" s="16"/>
+      <c r="H141" s="16"/>
+      <c r="I141" s="16"/>
+    </row>
+    <row r="142" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B142" s="8">
+        <v>13</v>
+      </c>
+      <c r="C142" s="9">
+        <v>14</v>
+      </c>
+      <c r="D142" s="9">
+        <v>2</v>
+      </c>
+      <c r="E142" s="101" t="s">
+        <v>67</v>
+      </c>
+      <c r="F142" s="95"/>
+      <c r="G142" s="16"/>
+      <c r="H142" s="16"/>
+      <c r="I142" s="16"/>
+    </row>
+    <row r="143" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B143" s="8">
+        <v>15</v>
+      </c>
+      <c r="C143" s="9">
+        <v>15</v>
+      </c>
+      <c r="D143" s="9">
+        <v>1</v>
+      </c>
+      <c r="E143" s="101" t="s">
+        <v>68</v>
+      </c>
+      <c r="F143" s="95"/>
+      <c r="G143" s="16"/>
+      <c r="H143" s="16"/>
+      <c r="I143" s="16"/>
+    </row>
+    <row r="144" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B144" s="8">
+        <v>16</v>
+      </c>
+      <c r="C144" s="9">
+        <v>19</v>
+      </c>
+      <c r="D144" s="9">
+        <v>4</v>
+      </c>
+      <c r="E144" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="F144" s="95"/>
+      <c r="G144" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="H144" s="16"/>
+      <c r="I144" s="16"/>
+    </row>
+    <row r="145" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B145" s="8">
+        <v>20</v>
+      </c>
+      <c r="C145" s="9">
+        <v>20</v>
+      </c>
+      <c r="D145" s="9">
+        <v>1</v>
+      </c>
+      <c r="E145" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="F145" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="G145" s="16"/>
+      <c r="H145" s="16"/>
+      <c r="I145" s="16"/>
+    </row>
+    <row r="146" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B146" s="8">
+        <v>21</v>
+      </c>
+      <c r="C146" s="9">
+        <v>22</v>
+      </c>
+      <c r="D146" s="9">
+        <v>2</v>
+      </c>
+      <c r="E146" s="101" t="s">
+        <v>71</v>
+      </c>
+      <c r="F146" s="95"/>
+      <c r="G146" s="16"/>
+      <c r="H146" s="16"/>
+      <c r="I146" s="16"/>
+    </row>
+    <row r="147" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B147" s="8">
+        <v>23</v>
+      </c>
+      <c r="C147" s="9">
+        <v>24</v>
+      </c>
+      <c r="D147" s="9">
+        <v>2</v>
+      </c>
+      <c r="E147" s="101" t="s">
+        <v>72</v>
+      </c>
+      <c r="F147" s="95"/>
+      <c r="G147" s="16"/>
+      <c r="H147" s="16"/>
+      <c r="I147" s="16"/>
+    </row>
+    <row r="148" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B148" s="8">
+        <v>25</v>
+      </c>
+      <c r="C148" s="9">
+        <v>26</v>
+      </c>
+      <c r="D148" s="9">
+        <v>2</v>
+      </c>
+      <c r="E148" s="101" t="s">
+        <v>73</v>
+      </c>
+      <c r="F148" s="95"/>
+      <c r="G148" s="16"/>
+      <c r="H148" s="16"/>
+      <c r="I148" s="16"/>
+    </row>
+    <row r="149" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B149" s="8">
+        <v>27</v>
+      </c>
+      <c r="C149" s="9">
+        <v>28</v>
+      </c>
+      <c r="D149" s="9">
+        <v>2</v>
+      </c>
+      <c r="E149" s="101" t="s">
+        <v>74</v>
+      </c>
+      <c r="F149" s="95"/>
+      <c r="G149" s="16"/>
+      <c r="H149" s="16"/>
+      <c r="I149" s="16"/>
+    </row>
+    <row r="150" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B150" s="8">
+        <v>29</v>
+      </c>
+      <c r="C150" s="9">
+        <v>32</v>
+      </c>
+      <c r="D150" s="9">
+        <v>4</v>
+      </c>
+      <c r="E150" s="101" t="s">
+        <v>75</v>
+      </c>
+      <c r="F150" s="95"/>
+      <c r="G150" s="16"/>
+      <c r="H150" s="16"/>
+      <c r="I150" s="16"/>
+    </row>
+    <row r="151" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B151" s="8">
+        <v>33</v>
+      </c>
+      <c r="C151" s="9">
+        <v>36</v>
+      </c>
+      <c r="D151" s="9">
+        <v>4</v>
+      </c>
+      <c r="E151" s="101" t="s">
+        <v>76</v>
+      </c>
+      <c r="F151" s="95"/>
+      <c r="G151" s="16"/>
+      <c r="H151" s="16"/>
+      <c r="I151" s="16"/>
+    </row>
+    <row r="152" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B152" s="8">
+        <v>37</v>
+      </c>
+      <c r="C152" s="9">
+        <v>38</v>
+      </c>
+      <c r="D152" s="9">
+        <v>2</v>
+      </c>
+      <c r="E152" s="101" t="s">
         <v>77</v>
       </c>
-      <c r="B78" s="49" t="s">
-        <v>135</v>
-      </c>
-      <c r="C78" s="50" t="s">
-        <v>136</v>
-      </c>
-      <c r="D78" s="50">
-        <v>1</v>
-      </c>
-      <c r="E78" s="50" t="s">
-        <v>137</v>
-      </c>
-      <c r="F78" s="37" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="79" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="B79" s="49" t="s">
-        <v>139</v>
-      </c>
-      <c r="C79" s="50" t="s">
-        <v>140</v>
-      </c>
-      <c r="D79" s="50">
-        <v>2</v>
-      </c>
-      <c r="E79" s="64" t="s">
-        <v>141</v>
-      </c>
-      <c r="F79" s="26"/>
-    </row>
-    <row r="80" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="B80" s="49" t="s">
-        <v>142</v>
-      </c>
-      <c r="C80" s="50" t="s">
-        <v>143</v>
-      </c>
-      <c r="D80" s="50">
-        <v>2</v>
-      </c>
-      <c r="E80" s="64" t="s">
-        <v>144</v>
-      </c>
-      <c r="F80" s="26"/>
-    </row>
-    <row r="81" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="B81" s="49" t="s">
-        <v>145</v>
-      </c>
-      <c r="C81" s="50" t="s">
-        <v>146</v>
-      </c>
-      <c r="D81" s="50">
-        <v>2</v>
-      </c>
-      <c r="E81" s="64" t="s">
-        <v>147</v>
-      </c>
-      <c r="F81" s="26"/>
-    </row>
-    <row r="82" spans="1:6" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="B82" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="C82" s="48" t="s">
-        <v>149</v>
-      </c>
-      <c r="D82" s="48">
-        <v>2</v>
-      </c>
-      <c r="E82" s="53" t="s">
-        <v>150</v>
-      </c>
-      <c r="F82" s="27"/>
-    </row>
-    <row r="83" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B85" s="77" t="s">
-        <v>81</v>
-      </c>
-      <c r="C85" s="77"/>
-      <c r="D85" s="77"/>
-      <c r="E85" s="77"/>
-      <c r="F85" s="77"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B86" s="77"/>
-      <c r="C86" s="77"/>
-      <c r="D86" s="77"/>
-      <c r="E86" s="77"/>
-      <c r="F86" s="77"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B87" s="77"/>
-      <c r="C87" s="77"/>
-      <c r="D87" s="77"/>
-      <c r="E87" s="77"/>
-      <c r="F87" s="77"/>
+      <c r="F152" s="95"/>
+      <c r="G152" s="16"/>
+      <c r="H152" s="16"/>
+      <c r="I152" s="16"/>
+    </row>
+    <row r="153" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B153" s="8">
+        <v>39</v>
+      </c>
+      <c r="C153" s="9">
+        <v>40</v>
+      </c>
+      <c r="D153" s="9">
+        <v>2</v>
+      </c>
+      <c r="E153" s="101" t="s">
+        <v>78</v>
+      </c>
+      <c r="F153" s="95"/>
+      <c r="G153" s="16"/>
+      <c r="H153" s="16"/>
+      <c r="I153" s="16"/>
+    </row>
+    <row r="154" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B154" s="8">
+        <v>41</v>
+      </c>
+      <c r="C154" s="9">
+        <v>48</v>
+      </c>
+      <c r="D154" s="9">
+        <v>8</v>
+      </c>
+      <c r="E154" s="101" t="s">
+        <v>78</v>
+      </c>
+      <c r="F154" s="95"/>
+      <c r="G154" s="16"/>
+      <c r="H154" s="16"/>
+      <c r="I154" s="16"/>
+    </row>
+    <row r="155" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B155" s="8">
+        <v>49</v>
+      </c>
+      <c r="C155" s="9">
+        <v>52</v>
+      </c>
+      <c r="D155" s="9">
+        <v>4</v>
+      </c>
+      <c r="E155" s="101" t="s">
+        <v>79</v>
+      </c>
+      <c r="F155" s="95"/>
+      <c r="G155" s="16"/>
+      <c r="H155" s="16"/>
+      <c r="I155" s="16"/>
+    </row>
+    <row r="156" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B156" s="8">
+        <v>53</v>
+      </c>
+      <c r="C156" s="9">
+        <v>56</v>
+      </c>
+      <c r="D156" s="9">
+        <v>4</v>
+      </c>
+      <c r="E156" s="101" t="s">
+        <v>80</v>
+      </c>
+      <c r="F156" s="95"/>
+      <c r="G156" s="16"/>
+      <c r="H156" s="16"/>
+      <c r="I156" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="56">
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
+  <mergeCells count="82">
+    <mergeCell ref="E155:F155"/>
+    <mergeCell ref="E156:F156"/>
+    <mergeCell ref="E150:F150"/>
+    <mergeCell ref="E151:F151"/>
+    <mergeCell ref="E152:F152"/>
+    <mergeCell ref="E153:F153"/>
+    <mergeCell ref="E154:F154"/>
+    <mergeCell ref="E144:F144"/>
+    <mergeCell ref="E146:F146"/>
+    <mergeCell ref="E147:F147"/>
+    <mergeCell ref="E148:F148"/>
+    <mergeCell ref="E149:F149"/>
+    <mergeCell ref="E139:F139"/>
+    <mergeCell ref="E140:F140"/>
+    <mergeCell ref="E141:F141"/>
+    <mergeCell ref="E142:F142"/>
+    <mergeCell ref="E143:F143"/>
+    <mergeCell ref="B133:C133"/>
+    <mergeCell ref="E133:F133"/>
+    <mergeCell ref="E134:F134"/>
+    <mergeCell ref="E137:F137"/>
+    <mergeCell ref="E138:F138"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="E73:F73"/>
     <mergeCell ref="E58:F58"/>
     <mergeCell ref="E59:F59"/>
-    <mergeCell ref="B85:F87"/>
+    <mergeCell ref="B99:F101"/>
     <mergeCell ref="L42:S42"/>
     <mergeCell ref="B61:F61"/>
     <mergeCell ref="L72:N72"/>
@@ -4036,11 +5186,45 @@
     <mergeCell ref="E49:F49"/>
     <mergeCell ref="E50:F50"/>
     <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="J79:M79"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
very important scripts to change MILL and IPS day to up to date CDC or System Date (IPS does not have CDC concept nor does have checksum)
</commit_message>
<xml_diff>
--- a/New Terminals/Sign-on/Sign-On.xlsx
+++ b/New Terminals/Sign-on/Sign-On.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\105864\Documents\Millennium\New Terminals\Sign-on\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4988D1AC-8970-4C86-81D6-113F7F735AE4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C725484A-BA98-4502-8E93-8E86B0973B0C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A59DBA4C-956A-4B57-A1C8-C87C01DAE8BE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="262">
   <si>
     <r>
       <t>Test</t>
@@ -858,28 +858,6 @@
     <t>0110 = X04+X02</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x0004 = Control Rev. Present -&gt; 2 (bytes to follow)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                                                                  x0002 = Text Rev. Present -&gt; 2 (bytes to follow)</t>
-    </r>
-  </si>
-  <si>
     <t>74-75</t>
   </si>
   <si>
@@ -890,13 +868,19 @@
   </si>
   <si>
     <t>Games</t>
+  </si>
+  <si>
+    <t>x0004 = Control Rev. Present -&gt; 2 (bytes to follow)                                                                  x0002 = Text Rev. Present -&gt; 2 (bytes to follow)</t>
+  </si>
+  <si>
+    <t>497</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -947,13 +931,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1468,7 +1445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1571,9 +1548,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1675,14 +1649,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1741,46 +1709,32 @@
     <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1801,6 +1755,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1813,7 +1785,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2311,8 +2282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4A5A7B-0DA8-401C-B426-04429DCC05B9}">
   <dimension ref="A2:S156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G76" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N85" sqref="N85"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I91" sqref="I91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2332,25 +2303,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
     </row>
     <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="2:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="102" t="s">
+      <c r="B4" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="103"/>
+      <c r="C4" s="108"/>
       <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="104" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="105"/>
+      <c r="E4" s="109" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="110"/>
       <c r="G4" s="12" t="s">
         <v>24</v>
       </c>
@@ -2369,8 +2340,8 @@
         <v>4</v>
       </c>
       <c r="D5" s="5"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="107"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="112"/>
     </row>
     <row r="6" spans="2:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="6">
@@ -2440,10 +2411,10 @@
       <c r="D8" s="9">
         <v>2</v>
       </c>
-      <c r="E8" s="108" t="s">
+      <c r="E8" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="109"/>
+      <c r="F8" s="102"/>
       <c r="G8" s="12" t="s">
         <v>30</v>
       </c>
@@ -2467,10 +2438,10 @@
       <c r="D9" s="9">
         <v>1</v>
       </c>
-      <c r="E9" s="101" t="s">
+      <c r="E9" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="95"/>
+      <c r="F9" s="100"/>
       <c r="G9" s="16" t="s">
         <v>39</v>
       </c>
@@ -2492,10 +2463,10 @@
       <c r="D10" s="9">
         <v>4</v>
       </c>
-      <c r="E10" s="101" t="s">
+      <c r="E10" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="95"/>
+      <c r="F10" s="100"/>
       <c r="G10" s="19" t="s">
         <v>37</v>
       </c>
@@ -2519,10 +2490,10 @@
       <c r="D11" s="9">
         <v>2</v>
       </c>
-      <c r="E11" s="101" t="s">
+      <c r="E11" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="95"/>
+      <c r="F11" s="100"/>
       <c r="G11" s="20" t="s">
         <v>38</v>
       </c>
@@ -2546,10 +2517,10 @@
       <c r="D12" s="9">
         <v>2</v>
       </c>
-      <c r="E12" s="101" t="s">
+      <c r="E12" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="95"/>
+      <c r="F12" s="100"/>
       <c r="G12" s="19" t="s">
         <v>42</v>
       </c>
@@ -2573,10 +2544,10 @@
       <c r="D13" s="9">
         <v>8</v>
       </c>
-      <c r="E13" s="101" t="s">
+      <c r="E13" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="95"/>
+      <c r="F13" s="100"/>
       <c r="G13" s="20" t="s">
         <v>46</v>
       </c>
@@ -2600,10 +2571,10 @@
       <c r="D14" s="9">
         <v>8</v>
       </c>
-      <c r="E14" s="101" t="s">
+      <c r="E14" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="95"/>
+      <c r="F14" s="100"/>
       <c r="G14" s="16" t="s">
         <v>48</v>
       </c>
@@ -2625,10 +2596,10 @@
       <c r="D15" s="9">
         <v>8</v>
       </c>
-      <c r="E15" s="101" t="s">
+      <c r="E15" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="95"/>
+      <c r="F15" s="100"/>
       <c r="G15" s="19" t="s">
         <v>46</v>
       </c>
@@ -2652,10 +2623,10 @@
       <c r="D16" s="9">
         <v>8</v>
       </c>
-      <c r="E16" s="101" t="s">
+      <c r="E16" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="95"/>
+      <c r="F16" s="100"/>
       <c r="G16" s="19" t="s">
         <v>46</v>
       </c>
@@ -2679,10 +2650,10 @@
       <c r="D17" s="9">
         <v>8</v>
       </c>
-      <c r="E17" s="101" t="s">
+      <c r="E17" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="95"/>
+      <c r="F17" s="100"/>
       <c r="G17" s="19" t="s">
         <v>46</v>
       </c>
@@ -2706,10 +2677,10 @@
       <c r="D18" s="9">
         <v>8</v>
       </c>
-      <c r="E18" s="101" t="s">
+      <c r="E18" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="95"/>
+      <c r="F18" s="100"/>
       <c r="G18" s="19" t="s">
         <v>46</v>
       </c>
@@ -2733,10 +2704,10 @@
       <c r="D19" s="9">
         <v>4</v>
       </c>
-      <c r="E19" s="101" t="s">
+      <c r="E19" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="95"/>
+      <c r="F19" s="100"/>
       <c r="G19" s="19" t="s">
         <v>50</v>
       </c>
@@ -2760,10 +2731,10 @@
       <c r="D20" s="9">
         <v>4</v>
       </c>
-      <c r="E20" s="101" t="s">
+      <c r="E20" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="95"/>
+      <c r="F20" s="100"/>
       <c r="G20" s="16" t="s">
         <v>51</v>
       </c>
@@ -2787,10 +2758,10 @@
       <c r="D21" s="9">
         <v>4</v>
       </c>
-      <c r="E21" s="101" t="s">
+      <c r="E21" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="95"/>
+      <c r="F21" s="100"/>
       <c r="G21" s="16" t="s">
         <v>52</v>
       </c>
@@ -2814,10 +2785,10 @@
       <c r="D22" s="9">
         <v>4</v>
       </c>
-      <c r="E22" s="101" t="s">
+      <c r="E22" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="95"/>
+      <c r="F22" s="100"/>
       <c r="G22" s="16" t="s">
         <v>50</v>
       </c>
@@ -2841,10 +2812,10 @@
       <c r="D23" s="9">
         <v>4</v>
       </c>
-      <c r="E23" s="101" t="s">
+      <c r="E23" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="95"/>
+      <c r="F23" s="100"/>
       <c r="G23" s="24" t="s">
         <v>54</v>
       </c>
@@ -2868,10 +2839,10 @@
       <c r="D24" s="9">
         <v>4</v>
       </c>
-      <c r="E24" s="101" t="s">
+      <c r="E24" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="95"/>
+      <c r="F24" s="100"/>
       <c r="G24" s="19" t="s">
         <v>53</v>
       </c>
@@ -2895,10 +2866,10 @@
       <c r="D25" s="9">
         <v>4</v>
       </c>
-      <c r="E25" s="101" t="s">
+      <c r="E25" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="95"/>
+      <c r="F25" s="100"/>
       <c r="G25" s="19" t="s">
         <v>53</v>
       </c>
@@ -2922,10 +2893,10 @@
       <c r="D26" s="9">
         <v>4</v>
       </c>
-      <c r="E26" s="101" t="s">
+      <c r="E26" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="95"/>
+      <c r="F26" s="100"/>
       <c r="G26" s="19" t="s">
         <v>50</v>
       </c>
@@ -2949,10 +2920,10 @@
       <c r="D27" s="9">
         <v>4</v>
       </c>
-      <c r="E27" s="101" t="s">
+      <c r="E27" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="F27" s="95"/>
+      <c r="F27" s="100"/>
       <c r="G27" s="19" t="s">
         <v>50</v>
       </c>
@@ -2976,10 +2947,10 @@
       <c r="D28" s="9">
         <v>4</v>
       </c>
-      <c r="E28" s="101" t="s">
+      <c r="E28" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="F28" s="95"/>
+      <c r="F28" s="100"/>
       <c r="G28" s="19" t="s">
         <v>50</v>
       </c>
@@ -3003,10 +2974,10 @@
       <c r="D29" s="9">
         <v>4</v>
       </c>
-      <c r="E29" s="101" t="s">
+      <c r="E29" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="95"/>
+      <c r="F29" s="100"/>
       <c r="G29" s="19" t="s">
         <v>50</v>
       </c>
@@ -3030,10 +3001,10 @@
       <c r="D30" s="11">
         <v>4</v>
       </c>
-      <c r="E30" s="110" t="s">
+      <c r="E30" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="F30" s="111"/>
+      <c r="F30" s="104"/>
       <c r="G30" s="19" t="s">
         <v>50</v>
       </c>
@@ -3160,10 +3131,10 @@
       <c r="D40" s="9">
         <v>2</v>
       </c>
-      <c r="E40" s="108" t="s">
+      <c r="E40" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="F40" s="109"/>
+      <c r="F40" s="102"/>
       <c r="G40" s="16" t="s">
         <v>82</v>
       </c>
@@ -3184,10 +3155,10 @@
       <c r="D41" s="9">
         <v>3</v>
       </c>
-      <c r="E41" s="101" t="s">
+      <c r="E41" s="99" t="s">
         <v>63</v>
       </c>
-      <c r="F41" s="95"/>
+      <c r="F41" s="100"/>
       <c r="G41" s="19" t="s">
         <v>85</v>
       </c>
@@ -3197,7 +3168,7 @@
       <c r="I41" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="J41" s="37" t="s">
+      <c r="J41" s="36" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3211,10 +3182,10 @@
       <c r="D42" s="9">
         <v>2</v>
       </c>
-      <c r="E42" s="101" t="s">
+      <c r="E42" s="99" t="s">
         <v>64</v>
       </c>
-      <c r="F42" s="95"/>
+      <c r="F42" s="100"/>
       <c r="G42" s="19" t="s">
         <v>89</v>
       </c>
@@ -3227,14 +3198,14 @@
       <c r="J42" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="L42" s="115"/>
-      <c r="M42" s="115"/>
-      <c r="N42" s="115"/>
-      <c r="O42" s="115"/>
-      <c r="P42" s="115"/>
-      <c r="Q42" s="115"/>
-      <c r="R42" s="115"/>
-      <c r="S42" s="115"/>
+      <c r="L42" s="114"/>
+      <c r="M42" s="114"/>
+      <c r="N42" s="114"/>
+      <c r="O42" s="114"/>
+      <c r="P42" s="114"/>
+      <c r="Q42" s="114"/>
+      <c r="R42" s="114"/>
+      <c r="S42" s="114"/>
     </row>
     <row r="43" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B43" s="8">
@@ -3246,10 +3217,10 @@
       <c r="D43" s="9">
         <v>2</v>
       </c>
-      <c r="E43" s="101" t="s">
+      <c r="E43" s="99" t="s">
         <v>65</v>
       </c>
-      <c r="F43" s="95"/>
+      <c r="F43" s="100"/>
       <c r="G43" s="16" t="s">
         <v>93</v>
       </c>
@@ -3273,20 +3244,20 @@
       <c r="D44" s="9">
         <v>1</v>
       </c>
-      <c r="E44" s="101" t="s">
+      <c r="E44" s="99" t="s">
         <v>66</v>
       </c>
-      <c r="F44" s="95"/>
-      <c r="G44" s="60" t="s">
+      <c r="F44" s="100"/>
+      <c r="G44" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="H44" s="60" t="s">
+      <c r="H44" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="I44" s="60" t="s">
+      <c r="I44" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="J44" s="61" t="s">
+      <c r="J44" s="60" t="s">
         <v>99</v>
       </c>
     </row>
@@ -3300,10 +3271,10 @@
       <c r="D45" s="9">
         <v>2</v>
       </c>
-      <c r="E45" s="101" t="s">
+      <c r="E45" s="99" t="s">
         <v>67</v>
       </c>
-      <c r="F45" s="95"/>
+      <c r="F45" s="100"/>
       <c r="G45" s="12" t="s">
         <v>100</v>
       </c>
@@ -3313,7 +3284,7 @@
       <c r="I45" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="J45" s="38" t="s">
+      <c r="J45" s="37" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3327,10 +3298,10 @@
       <c r="D46" s="9">
         <v>1</v>
       </c>
-      <c r="E46" s="101" t="s">
+      <c r="E46" s="99" t="s">
         <v>68</v>
       </c>
-      <c r="F46" s="95"/>
+      <c r="F46" s="100"/>
       <c r="G46" s="19" t="s">
         <v>104</v>
       </c>
@@ -3340,7 +3311,7 @@
       <c r="I46" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="J46" s="37" t="s">
+      <c r="J46" s="36" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3354,10 +3325,10 @@
       <c r="D47" s="9">
         <v>4</v>
       </c>
-      <c r="E47" s="101" t="s">
+      <c r="E47" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="95"/>
+      <c r="F47" s="100"/>
       <c r="G47" s="18" t="s">
         <v>37</v>
       </c>
@@ -3381,26 +3352,26 @@
       <c r="D48" s="9">
         <v>1</v>
       </c>
-      <c r="E48" s="36" t="s">
+      <c r="E48" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="F48" s="36" t="s">
+      <c r="F48" s="35" t="s">
         <v>70</v>
       </c>
       <c r="G48" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="H48" s="39" t="s">
+      <c r="H48" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="I48" s="39" t="s">
+      <c r="I48" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="J48" s="40" t="s">
+      <c r="J48" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="K48" s="41"/>
-      <c r="L48" s="42" t="s">
+      <c r="K48" s="40"/>
+      <c r="L48" s="41" t="s">
         <v>114</v>
       </c>
     </row>
@@ -3414,10 +3385,10 @@
       <c r="D49" s="9">
         <v>2</v>
       </c>
-      <c r="E49" s="101" t="s">
+      <c r="E49" s="99" t="s">
         <v>71</v>
       </c>
-      <c r="F49" s="95"/>
+      <c r="F49" s="100"/>
       <c r="G49" s="19" t="s">
         <v>116</v>
       </c>
@@ -3427,7 +3398,7 @@
       <c r="I49" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="J49" s="43" t="s">
+      <c r="J49" s="42" t="s">
         <v>119</v>
       </c>
     </row>
@@ -3441,10 +3412,10 @@
       <c r="D50" s="9">
         <v>2</v>
       </c>
-      <c r="E50" s="101" t="s">
+      <c r="E50" s="99" t="s">
         <v>72</v>
       </c>
-      <c r="F50" s="95"/>
+      <c r="F50" s="100"/>
       <c r="G50" s="16" t="s">
         <v>120</v>
       </c>
@@ -3465,10 +3436,10 @@
       <c r="D51" s="9">
         <v>2</v>
       </c>
-      <c r="E51" s="101" t="s">
+      <c r="E51" s="99" t="s">
         <v>73</v>
       </c>
-      <c r="F51" s="95"/>
+      <c r="F51" s="100"/>
       <c r="G51" s="16" t="s">
         <v>120</v>
       </c>
@@ -3489,10 +3460,10 @@
       <c r="D52" s="9">
         <v>2</v>
       </c>
-      <c r="E52" s="101" t="s">
+      <c r="E52" s="99" t="s">
         <v>74</v>
       </c>
-      <c r="F52" s="95"/>
+      <c r="F52" s="100"/>
       <c r="G52" s="16" t="s">
         <v>38</v>
       </c>
@@ -3516,10 +3487,10 @@
       <c r="D53" s="9">
         <v>4</v>
       </c>
-      <c r="E53" s="101" t="s">
+      <c r="E53" s="99" t="s">
         <v>75</v>
       </c>
-      <c r="F53" s="95"/>
+      <c r="F53" s="100"/>
       <c r="G53" s="19" t="s">
         <v>50</v>
       </c>
@@ -3543,10 +3514,10 @@
       <c r="D54" s="9">
         <v>4</v>
       </c>
-      <c r="E54" s="101" t="s">
+      <c r="E54" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="F54" s="95"/>
+      <c r="F54" s="100"/>
       <c r="G54" s="18" t="s">
         <v>121</v>
       </c>
@@ -3570,10 +3541,10 @@
       <c r="D55" s="9">
         <v>2</v>
       </c>
-      <c r="E55" s="101" t="s">
+      <c r="E55" s="99" t="s">
         <v>77</v>
       </c>
-      <c r="F55" s="95"/>
+      <c r="F55" s="100"/>
       <c r="G55" s="18" t="s">
         <v>122</v>
       </c>
@@ -3597,10 +3568,10 @@
       <c r="D56" s="9">
         <v>2</v>
       </c>
-      <c r="E56" s="101" t="s">
+      <c r="E56" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="F56" s="95"/>
+      <c r="F56" s="100"/>
       <c r="G56" s="19" t="s">
         <v>38</v>
       </c>
@@ -3610,7 +3581,7 @@
       <c r="I56" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="J56" s="37" t="s">
+      <c r="J56" s="36" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3624,10 +3595,10 @@
       <c r="D57" s="9">
         <v>8</v>
       </c>
-      <c r="E57" s="101" t="s">
+      <c r="E57" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="F57" s="95"/>
+      <c r="F57" s="100"/>
       <c r="G57" s="19" t="s">
         <v>46</v>
       </c>
@@ -3637,7 +3608,7 @@
       <c r="I57" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="J57" s="37" t="s">
+      <c r="J57" s="36" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3651,10 +3622,10 @@
       <c r="D58" s="9">
         <v>4</v>
       </c>
-      <c r="E58" s="101" t="s">
+      <c r="E58" s="99" t="s">
         <v>79</v>
       </c>
-      <c r="F58" s="95"/>
+      <c r="F58" s="100"/>
       <c r="G58" s="18" t="s">
         <v>125</v>
       </c>
@@ -3678,10 +3649,10 @@
       <c r="D59" s="9">
         <v>4</v>
       </c>
-      <c r="E59" s="101" t="s">
+      <c r="E59" s="99" t="s">
         <v>80</v>
       </c>
-      <c r="F59" s="95"/>
+      <c r="F59" s="100"/>
       <c r="G59" s="18" t="s">
         <v>130</v>
       </c>
@@ -3697,44 +3668,44 @@
     </row>
     <row r="60" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="61" spans="1:16" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B61" s="116" t="s">
+      <c r="B61" s="115" t="s">
         <v>151</v>
       </c>
-      <c r="C61" s="116"/>
-      <c r="D61" s="116"/>
-      <c r="E61" s="116"/>
-      <c r="F61" s="116"/>
-      <c r="L61" s="54" t="s">
+      <c r="C61" s="115"/>
+      <c r="D61" s="115"/>
+      <c r="E61" s="115"/>
+      <c r="F61" s="115"/>
+      <c r="L61" s="53" t="s">
         <v>167</v>
       </c>
-      <c r="M61" s="55" t="s">
+      <c r="M61" s="54" t="s">
         <v>168</v>
       </c>
-      <c r="N61" s="55" t="s">
+      <c r="N61" s="54" t="s">
         <v>169</v>
       </c>
-      <c r="O61" s="55" t="s">
+      <c r="O61" s="54" t="s">
         <v>170</v>
       </c>
-      <c r="P61" s="56" t="s">
+      <c r="P61" s="55" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="62" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B62" s="44">
+      <c r="B62" s="43">
         <v>57</v>
       </c>
-      <c r="C62" s="45">
+      <c r="C62" s="44">
         <v>57</v>
       </c>
-      <c r="D62" s="45">
+      <c r="D62" s="44">
         <v>1</v>
       </c>
-      <c r="E62" s="50" t="s">
+      <c r="E62" s="49" t="s">
         <v>133</v>
       </c>
-      <c r="F62" s="51"/>
-      <c r="G62" s="93" t="s">
+      <c r="F62" s="50"/>
+      <c r="G62" s="90" t="s">
         <v>157</v>
       </c>
       <c r="H62" s="19" t="s">
@@ -3746,33 +3717,33 @@
       <c r="J62" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="L62" s="65">
+      <c r="L62" s="64">
         <v>1</v>
       </c>
-      <c r="M62" s="66" t="s">
+      <c r="M62" s="65" t="s">
         <v>172</v>
       </c>
-      <c r="N62" s="67">
+      <c r="N62" s="66">
         <v>17</v>
       </c>
-      <c r="O62" s="67">
+      <c r="O62" s="66">
         <v>1</v>
       </c>
-      <c r="P62" s="68" t="s">
+      <c r="P62" s="67" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="63" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B63" s="46">
+      <c r="B63" s="45">
         <v>58</v>
       </c>
-      <c r="C63" s="47">
+      <c r="C63" s="46">
         <v>58</v>
       </c>
-      <c r="D63" s="47">
+      <c r="D63" s="46">
         <v>1</v>
       </c>
-      <c r="E63" s="52" t="s">
+      <c r="E63" s="51" t="s">
         <v>134</v>
       </c>
       <c r="F63" s="26"/>
@@ -3788,19 +3759,19 @@
       <c r="J63" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="L63" s="48">
-        <v>2</v>
-      </c>
-      <c r="M63" s="57" t="s">
+      <c r="L63" s="47">
+        <v>2</v>
+      </c>
+      <c r="M63" s="56" t="s">
         <v>174</v>
       </c>
-      <c r="N63" s="49">
+      <c r="N63" s="48">
         <v>19</v>
       </c>
-      <c r="O63" s="49">
-        <v>2</v>
-      </c>
-      <c r="P63" s="36" t="s">
+      <c r="O63" s="48">
+        <v>2</v>
+      </c>
+      <c r="P63" s="35" t="s">
         <v>175</v>
       </c>
     </row>
@@ -3808,19 +3779,19 @@
       <c r="A64" s="12">
         <v>59</v>
       </c>
-      <c r="B64" s="48" t="s">
+      <c r="B64" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="C64" s="49" t="s">
+      <c r="C64" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="D64" s="49">
+      <c r="D64" s="48">
         <v>1</v>
       </c>
-      <c r="E64" s="49" t="s">
+      <c r="E64" s="48" t="s">
         <v>137</v>
       </c>
-      <c r="F64" s="36" t="s">
+      <c r="F64" s="35" t="s">
         <v>138</v>
       </c>
       <c r="G64" s="19" t="s">
@@ -3832,42 +3803,42 @@
       <c r="I64" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="J64" s="64" t="s">
-        <v>258</v>
-      </c>
-      <c r="L64" s="48">
+      <c r="J64" s="63" t="s">
+        <v>257</v>
+      </c>
+      <c r="L64" s="47">
         <v>3</v>
       </c>
-      <c r="M64" s="57" t="s">
+      <c r="M64" s="56" t="s">
         <v>176</v>
       </c>
-      <c r="N64" s="49">
-        <v>2</v>
-      </c>
-      <c r="O64" s="49">
+      <c r="N64" s="48">
+        <v>2</v>
+      </c>
+      <c r="O64" s="48">
         <v>1</v>
       </c>
-      <c r="P64" s="36" t="s">
+      <c r="P64" s="35" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="65" spans="1:16" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="12" t="s">
+      <c r="A65" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="B65" s="48" t="s">
+      <c r="B65" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="C65" s="49" t="s">
+      <c r="C65" s="66" t="s">
         <v>140</v>
       </c>
-      <c r="D65" s="49">
-        <v>2</v>
-      </c>
-      <c r="E65" s="94" t="s">
+      <c r="D65" s="66">
+        <v>2</v>
+      </c>
+      <c r="E65" s="92" t="s">
         <v>141</v>
       </c>
-      <c r="F65" s="95"/>
+      <c r="F65" s="93"/>
       <c r="G65" s="19" t="s">
         <v>164</v>
       </c>
@@ -3880,84 +3851,84 @@
       <c r="J65" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="L65" s="48">
+      <c r="L65" s="47">
         <v>4</v>
       </c>
-      <c r="M65" s="57" t="s">
+      <c r="M65" s="56" t="s">
         <v>178</v>
       </c>
-      <c r="N65" s="49">
+      <c r="N65" s="48">
         <v>4</v>
       </c>
-      <c r="O65" s="49">
+      <c r="O65" s="48">
         <v>1</v>
       </c>
-      <c r="P65" s="36" t="s">
+      <c r="P65" s="35" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="66" spans="1:16" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="12" t="s">
+      <c r="A66" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="B66" s="48" t="s">
+      <c r="B66" s="64" t="s">
         <v>142</v>
       </c>
-      <c r="C66" s="49" t="s">
+      <c r="C66" s="66" t="s">
         <v>143</v>
       </c>
-      <c r="D66" s="49">
-        <v>2</v>
-      </c>
-      <c r="E66" s="94" t="s">
+      <c r="D66" s="66">
+        <v>2</v>
+      </c>
+      <c r="E66" s="92" t="s">
         <v>144</v>
       </c>
-      <c r="F66" s="95"/>
-      <c r="G66" s="16" t="s">
+      <c r="F66" s="93"/>
+      <c r="G66" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="H66" s="16" t="s">
+      <c r="H66" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="I66" s="16" t="s">
+      <c r="I66" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="J66" s="12" t="s">
+      <c r="J66" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="L66" s="48">
+      <c r="L66" s="47">
         <v>5</v>
       </c>
-      <c r="M66" s="57" t="s">
+      <c r="M66" s="56" t="s">
         <v>180</v>
       </c>
-      <c r="N66" s="49">
+      <c r="N66" s="48">
         <v>1</v>
       </c>
-      <c r="O66" s="49">
+      <c r="O66" s="48">
         <v>3</v>
       </c>
-      <c r="P66" s="36" t="s">
+      <c r="P66" s="35" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="67" spans="1:16" s="82" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="63" t="s">
+    <row r="67" spans="1:16" s="79" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="62" t="s">
         <v>192</v>
       </c>
-      <c r="B67" s="73" t="s">
+      <c r="B67" s="70" t="s">
         <v>145</v>
       </c>
-      <c r="C67" s="74" t="s">
+      <c r="C67" s="71" t="s">
         <v>146</v>
       </c>
-      <c r="D67" s="74">
-        <v>2</v>
-      </c>
-      <c r="E67" s="96" t="s">
+      <c r="D67" s="71">
+        <v>2</v>
+      </c>
+      <c r="E67" s="94" t="s">
         <v>147</v>
       </c>
-      <c r="F67" s="97"/>
+      <c r="F67" s="95"/>
       <c r="G67" s="24" t="s">
         <v>195</v>
       </c>
@@ -3967,43 +3938,43 @@
       <c r="I67" s="24" t="s">
         <v>196</v>
       </c>
-      <c r="J67" s="63" t="s">
+      <c r="J67" s="62" t="s">
         <v>194</v>
       </c>
-      <c r="L67" s="80">
+      <c r="L67" s="77">
         <v>6</v>
       </c>
-      <c r="M67" s="83" t="s">
+      <c r="M67" s="80" t="s">
         <v>182</v>
       </c>
-      <c r="N67" s="81">
+      <c r="N67" s="78">
         <v>1</v>
       </c>
-      <c r="O67" s="81">
+      <c r="O67" s="78">
         <v>4</v>
       </c>
-      <c r="P67" s="84" t="s">
+      <c r="P67" s="81" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="68" spans="1:16" s="82" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="63" t="s">
+    <row r="68" spans="1:16" s="79" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="62" t="s">
         <v>193</v>
       </c>
-      <c r="B68" s="75" t="s">
+      <c r="B68" s="72" t="s">
         <v>148</v>
       </c>
-      <c r="C68" s="76" t="s">
+      <c r="C68" s="73" t="s">
         <v>149</v>
       </c>
-      <c r="D68" s="76">
-        <v>2</v>
-      </c>
-      <c r="E68" s="98" t="s">
+      <c r="D68" s="73">
+        <v>2</v>
+      </c>
+      <c r="E68" s="96" t="s">
         <v>150</v>
       </c>
-      <c r="F68" s="99"/>
-      <c r="G68" s="63" t="s">
+      <c r="F68" s="97"/>
+      <c r="G68" s="62" t="s">
         <v>198</v>
       </c>
       <c r="H68" s="24" t="s">
@@ -4012,20 +3983,20 @@
       <c r="I68" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="J68" s="63"/>
-      <c r="L68" s="80">
+      <c r="J68" s="62"/>
+      <c r="L68" s="77">
         <v>7</v>
       </c>
-      <c r="M68" s="83" t="s">
+      <c r="M68" s="80" t="s">
         <v>184</v>
       </c>
-      <c r="N68" s="81">
+      <c r="N68" s="78">
         <v>16</v>
       </c>
-      <c r="O68" s="81">
+      <c r="O68" s="78">
         <v>1</v>
       </c>
-      <c r="P68" s="84" t="s">
+      <c r="P68" s="81" t="s">
         <v>185</v>
       </c>
     </row>
@@ -4033,45 +4004,45 @@
       <c r="H69" s="12"/>
       <c r="I69" s="12"/>
       <c r="J69" s="12"/>
-      <c r="L69" s="48">
+      <c r="L69" s="47">
         <v>8</v>
       </c>
-      <c r="M69" s="57" t="s">
+      <c r="M69" s="56" t="s">
         <v>186</v>
       </c>
-      <c r="N69" s="49">
+      <c r="N69" s="48">
         <v>16</v>
       </c>
-      <c r="O69" s="49">
-        <v>2</v>
-      </c>
-      <c r="P69" s="36" t="s">
+      <c r="O69" s="48">
+        <v>2</v>
+      </c>
+      <c r="P69" s="35" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:16" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="62" t="s">
+      <c r="A70" s="61" t="s">
         <v>206</v>
       </c>
-      <c r="B70" s="63" t="s">
+      <c r="B70" s="62" t="s">
         <v>205</v>
       </c>
-      <c r="G70" s="63" t="s">
+      <c r="G70" s="62" t="s">
         <v>207</v>
       </c>
-      <c r="L70" s="46">
+      <c r="L70" s="45">
         <v>9</v>
       </c>
-      <c r="M70" s="58" t="s">
+      <c r="M70" s="57" t="s">
         <v>188</v>
       </c>
-      <c r="N70" s="47">
-        <v>2</v>
-      </c>
-      <c r="O70" s="47">
+      <c r="N70" s="46">
+        <v>2</v>
+      </c>
+      <c r="O70" s="46">
         <v>3</v>
       </c>
-      <c r="P70" s="59" t="s">
+      <c r="P70" s="58" t="s">
         <v>189</v>
       </c>
     </row>
@@ -4080,19 +4051,19 @@
       <c r="A72" s="18">
         <v>64</v>
       </c>
-      <c r="B72" s="65" t="s">
+      <c r="B72" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="C72" s="67" t="s">
+      <c r="C72" s="66" t="s">
         <v>136</v>
       </c>
-      <c r="D72" s="67">
+      <c r="D72" s="66">
         <v>1</v>
       </c>
-      <c r="E72" s="67" t="s">
+      <c r="E72" s="66" t="s">
         <v>137</v>
       </c>
-      <c r="F72" s="68" t="s">
+      <c r="F72" s="67" t="s">
         <v>138</v>
       </c>
       <c r="G72" s="19" t="s">
@@ -4104,149 +4075,149 @@
       <c r="I72" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="J72" s="64" t="s">
+      <c r="J72" s="63" t="s">
         <v>231</v>
       </c>
-      <c r="L72" s="117" t="s">
+      <c r="L72" s="116" t="s">
         <v>209</v>
       </c>
-      <c r="M72" s="117"/>
-      <c r="N72" s="117"/>
+      <c r="M72" s="116"/>
+      <c r="N72" s="116"/>
     </row>
     <row r="73" spans="1:16" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="12" t="s">
+      <c r="A73" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="B73" s="48" t="s">
+      <c r="B73" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="C73" s="49" t="s">
+      <c r="C73" s="66" t="s">
         <v>140</v>
       </c>
-      <c r="D73" s="49">
-        <v>2</v>
-      </c>
-      <c r="E73" s="94" t="s">
+      <c r="D73" s="66">
+        <v>2</v>
+      </c>
+      <c r="E73" s="92" t="s">
         <v>141</v>
       </c>
-      <c r="F73" s="95"/>
-      <c r="G73" s="16" t="s">
+      <c r="F73" s="93"/>
+      <c r="G73" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="H73" s="16" t="s">
+      <c r="H73" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="I73" s="16" t="s">
+      <c r="I73" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="J73" s="35" t="s">
+      <c r="J73" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="L73" s="117" t="s">
+      <c r="L73" s="116" t="s">
         <v>210</v>
       </c>
-      <c r="M73" s="117"/>
+      <c r="M73" s="116"/>
     </row>
     <row r="74" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="12" t="s">
+      <c r="A74" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="B74" s="48" t="s">
+      <c r="B74" s="64" t="s">
         <v>142</v>
       </c>
-      <c r="C74" s="49" t="s">
+      <c r="C74" s="66" t="s">
         <v>143</v>
       </c>
-      <c r="D74" s="49">
-        <v>2</v>
-      </c>
-      <c r="E74" s="94" t="s">
+      <c r="D74" s="66">
+        <v>2</v>
+      </c>
+      <c r="E74" s="92" t="s">
         <v>144</v>
       </c>
-      <c r="F74" s="95"/>
-      <c r="G74" s="16" t="s">
+      <c r="F74" s="93"/>
+      <c r="G74" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="H74" s="16" t="s">
+      <c r="H74" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="I74" s="16" t="s">
+      <c r="I74" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="J74" s="71" t="s">
+      <c r="J74" s="18" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="75" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="77" t="s">
+      <c r="A75" s="74" t="s">
         <v>201</v>
       </c>
-      <c r="B75" s="73" t="s">
+      <c r="B75" s="70" t="s">
         <v>145</v>
       </c>
-      <c r="C75" s="74" t="s">
+      <c r="C75" s="71" t="s">
         <v>146</v>
       </c>
-      <c r="D75" s="74">
-        <v>2</v>
-      </c>
-      <c r="E75" s="96" t="s">
+      <c r="D75" s="71">
+        <v>2</v>
+      </c>
+      <c r="E75" s="94" t="s">
         <v>147</v>
       </c>
-      <c r="F75" s="97"/>
-      <c r="G75" s="78"/>
-      <c r="H75" s="77"/>
-      <c r="I75" s="77"/>
-      <c r="J75" s="79"/>
-      <c r="K75" s="79"/>
+      <c r="F75" s="95"/>
+      <c r="G75" s="75"/>
+      <c r="H75" s="74"/>
+      <c r="I75" s="74"/>
+      <c r="J75" s="76"/>
+      <c r="K75" s="76"/>
     </row>
     <row r="76" spans="1:16" ht="26.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="77" t="s">
+      <c r="A76" s="74" t="s">
         <v>202</v>
       </c>
-      <c r="B76" s="75" t="s">
+      <c r="B76" s="72" t="s">
         <v>148</v>
       </c>
-      <c r="C76" s="76" t="s">
+      <c r="C76" s="73" t="s">
         <v>149</v>
       </c>
-      <c r="D76" s="76">
-        <v>2</v>
-      </c>
-      <c r="E76" s="98" t="s">
+      <c r="D76" s="73">
+        <v>2</v>
+      </c>
+      <c r="E76" s="96" t="s">
         <v>150</v>
       </c>
-      <c r="F76" s="99"/>
-      <c r="G76" s="78"/>
-      <c r="H76" s="77"/>
-      <c r="I76" s="77"/>
-      <c r="J76" s="79"/>
-      <c r="K76" s="79"/>
+      <c r="F76" s="97"/>
+      <c r="G76" s="75"/>
+      <c r="H76" s="74"/>
+      <c r="I76" s="74"/>
+      <c r="J76" s="76"/>
+      <c r="K76" s="76"/>
     </row>
     <row r="77" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="G77" s="89" t="s">
+      <c r="G77" s="86" t="s">
         <v>254</v>
       </c>
-      <c r="H77" s="71"/>
-      <c r="I77" s="71"/>
+      <c r="H77" s="69"/>
+      <c r="I77" s="69"/>
     </row>
     <row r="78" spans="1:16" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="18">
         <v>69</v>
       </c>
-      <c r="B78" s="65" t="s">
+      <c r="B78" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="C78" s="67" t="s">
+      <c r="C78" s="66" t="s">
         <v>136</v>
       </c>
-      <c r="D78" s="67">
+      <c r="D78" s="66">
         <v>1</v>
       </c>
-      <c r="E78" s="67" t="s">
+      <c r="E78" s="66" t="s">
         <v>137</v>
       </c>
-      <c r="F78" s="68" t="s">
+      <c r="F78" s="67" t="s">
         <v>138</v>
       </c>
       <c r="G78" s="19">
@@ -4266,19 +4237,19 @@
       <c r="A79" s="18" t="s">
         <v>236</v>
       </c>
-      <c r="B79" s="65" t="s">
+      <c r="B79" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="C79" s="67" t="s">
+      <c r="C79" s="66" t="s">
         <v>140</v>
       </c>
-      <c r="D79" s="67">
-        <v>2</v>
-      </c>
-      <c r="E79" s="90" t="s">
+      <c r="D79" s="66">
+        <v>2</v>
+      </c>
+      <c r="E79" s="87" t="s">
         <v>141</v>
       </c>
-      <c r="F79" s="91"/>
+      <c r="F79" s="88"/>
       <c r="G79" s="19" t="s">
         <v>238</v>
       </c>
@@ -4286,108 +4257,108 @@
         <v>255</v>
       </c>
       <c r="I79" s="19"/>
-      <c r="J79" s="100" t="s">
-        <v>256</v>
-      </c>
-      <c r="K79" s="100"/>
-      <c r="L79" s="100"/>
-      <c r="M79" s="100"/>
+      <c r="J79" s="98" t="s">
+        <v>260</v>
+      </c>
+      <c r="K79" s="98"/>
+      <c r="L79" s="98"/>
+      <c r="M79" s="98"/>
     </row>
     <row r="80" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="B80" s="65" t="s">
+      <c r="B80" s="64" t="s">
         <v>142</v>
       </c>
-      <c r="C80" s="67" t="s">
+      <c r="C80" s="66" t="s">
         <v>143</v>
       </c>
-      <c r="D80" s="67">
-        <v>2</v>
-      </c>
-      <c r="E80" s="90" t="s">
+      <c r="D80" s="66">
+        <v>2</v>
+      </c>
+      <c r="E80" s="87" t="s">
         <v>144</v>
       </c>
-      <c r="F80" s="91"/>
+      <c r="F80" s="88"/>
       <c r="G80" s="19" t="s">
         <v>239</v>
       </c>
       <c r="H80" s="19"/>
       <c r="I80" s="19"/>
-      <c r="J80" s="92"/>
-      <c r="K80" s="92"/>
-      <c r="L80" s="92"/>
-      <c r="M80" s="92"/>
+      <c r="J80" s="89"/>
+      <c r="K80" s="89"/>
+      <c r="L80" s="89"/>
+      <c r="M80" s="89"/>
     </row>
     <row r="81" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="18" t="s">
-        <v>257</v>
-      </c>
-      <c r="B81" s="65" t="s">
+        <v>256</v>
+      </c>
+      <c r="B81" s="64" t="s">
         <v>145</v>
       </c>
-      <c r="C81" s="67" t="s">
+      <c r="C81" s="66" t="s">
         <v>146</v>
       </c>
-      <c r="D81" s="67">
-        <v>2</v>
-      </c>
-      <c r="E81" s="90" t="s">
+      <c r="D81" s="66">
+        <v>2</v>
+      </c>
+      <c r="E81" s="87" t="s">
         <v>147</v>
       </c>
-      <c r="F81" s="91"/>
+      <c r="F81" s="88"/>
       <c r="G81" s="19" t="s">
         <v>242</v>
       </c>
       <c r="H81" s="19"/>
       <c r="I81" s="19"/>
-      <c r="J81" s="92"/>
+      <c r="J81" s="89"/>
     </row>
     <row r="82" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="63" t="s">
+      <c r="A82" s="62" t="s">
         <v>204</v>
       </c>
-      <c r="B82" s="75" t="s">
+      <c r="B82" s="72" t="s">
         <v>148</v>
       </c>
-      <c r="C82" s="76" t="s">
+      <c r="C82" s="73" t="s">
         <v>149</v>
       </c>
-      <c r="D82" s="76">
-        <v>2</v>
-      </c>
-      <c r="E82" s="87" t="s">
+      <c r="D82" s="73">
+        <v>2</v>
+      </c>
+      <c r="E82" s="84" t="s">
         <v>150</v>
       </c>
-      <c r="F82" s="88"/>
+      <c r="F82" s="85"/>
       <c r="G82" s="24"/>
       <c r="H82" s="24"/>
       <c r="I82" s="24"/>
-      <c r="J82" s="41"/>
+      <c r="J82" s="40"/>
     </row>
     <row r="83" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="L83" s="118" t="s">
-        <v>260</v>
+      <c r="L83" s="91" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="84" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="18">
         <v>74</v>
       </c>
-      <c r="B84" s="65" t="s">
+      <c r="B84" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="C84" s="67" t="s">
+      <c r="C84" s="66" t="s">
         <v>136</v>
       </c>
-      <c r="D84" s="67">
+      <c r="D84" s="66">
         <v>1</v>
       </c>
-      <c r="E84" s="67" t="s">
+      <c r="E84" s="66" t="s">
         <v>137</v>
       </c>
-      <c r="F84" s="68" t="s">
+      <c r="F84" s="67" t="s">
         <v>138</v>
       </c>
       <c r="G84" s="19" t="s">
@@ -4402,112 +4373,115 @@
       <c r="J84" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="L84" s="118" t="s">
+      <c r="L84" s="91" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="85" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="71" t="s">
+      <c r="A85" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="B85" s="48" t="s">
+      <c r="B85" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="C85" s="49" t="s">
+      <c r="C85" s="66" t="s">
         <v>140</v>
       </c>
-      <c r="D85" s="49">
-        <v>2</v>
-      </c>
-      <c r="E85" s="72" t="s">
+      <c r="D85" s="66">
+        <v>2</v>
+      </c>
+      <c r="E85" s="87" t="s">
         <v>141</v>
       </c>
-      <c r="F85" s="70"/>
-      <c r="G85" s="16" t="s">
+      <c r="F85" s="88"/>
+      <c r="G85" s="19" t="s">
         <v>247</v>
       </c>
-      <c r="H85" s="16"/>
-      <c r="I85" s="16"/>
-      <c r="J85" s="35" t="s">
+      <c r="H85" s="19"/>
+      <c r="I85" s="19"/>
+      <c r="J85" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="L85" s="118" t="s">
-        <v>259</v>
+      <c r="L85" s="91" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="86" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="71" t="s">
+      <c r="A86" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="B86" s="48" t="s">
+      <c r="B86" s="64" t="s">
         <v>142</v>
       </c>
-      <c r="C86" s="49" t="s">
+      <c r="C86" s="66" t="s">
         <v>143</v>
       </c>
-      <c r="D86" s="49">
-        <v>2</v>
-      </c>
-      <c r="E86" s="72" t="s">
+      <c r="D86" s="66">
+        <v>2</v>
+      </c>
+      <c r="E86" s="87" t="s">
         <v>144</v>
       </c>
-      <c r="F86" s="70"/>
-      <c r="G86" s="16" t="s">
+      <c r="F86" s="88"/>
+      <c r="G86" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="H86" s="16"/>
-      <c r="I86" s="16"/>
-      <c r="L86" s="118" t="s">
+      <c r="H86" s="19"/>
+      <c r="I86" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="J86" s="89"/>
+      <c r="L86" s="91" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="63" t="s">
+      <c r="A87" s="62" t="s">
         <v>203</v>
       </c>
-      <c r="B87" s="73" t="s">
+      <c r="B87" s="70" t="s">
         <v>145</v>
       </c>
-      <c r="C87" s="74" t="s">
+      <c r="C87" s="71" t="s">
         <v>146</v>
       </c>
-      <c r="D87" s="74">
-        <v>2</v>
-      </c>
-      <c r="E87" s="85" t="s">
+      <c r="D87" s="71">
+        <v>2</v>
+      </c>
+      <c r="E87" s="82" t="s">
         <v>147</v>
       </c>
-      <c r="F87" s="86"/>
+      <c r="F87" s="83"/>
       <c r="G87" s="24"/>
       <c r="H87" s="24"/>
       <c r="I87" s="24"/>
-      <c r="J87" s="41"/>
-      <c r="L87" s="118" t="s">
+      <c r="J87" s="40"/>
+      <c r="L87" s="91" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="88" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="63" t="s">
+      <c r="A88" s="62" t="s">
         <v>204</v>
       </c>
-      <c r="B88" s="75" t="s">
+      <c r="B88" s="72" t="s">
         <v>148</v>
       </c>
-      <c r="C88" s="76" t="s">
+      <c r="C88" s="73" t="s">
         <v>149</v>
       </c>
-      <c r="D88" s="76">
-        <v>2</v>
-      </c>
-      <c r="E88" s="87" t="s">
+      <c r="D88" s="73">
+        <v>2</v>
+      </c>
+      <c r="E88" s="84" t="s">
         <v>150</v>
       </c>
-      <c r="F88" s="88"/>
+      <c r="F88" s="85"/>
       <c r="G88" s="24"/>
       <c r="H88" s="24"/>
       <c r="I88" s="24"/>
-      <c r="J88" s="41"/>
-      <c r="L88" s="118" t="s">
+      <c r="J88" s="40"/>
+      <c r="L88" s="91" t="s">
         <v>182</v>
       </c>
     </row>
@@ -4516,19 +4490,19 @@
       <c r="A90" s="18">
         <v>79</v>
       </c>
-      <c r="B90" s="65" t="s">
+      <c r="B90" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="C90" s="67" t="s">
+      <c r="C90" s="66" t="s">
         <v>136</v>
       </c>
-      <c r="D90" s="67">
+      <c r="D90" s="66">
         <v>1</v>
       </c>
-      <c r="E90" s="67" t="s">
+      <c r="E90" s="66" t="s">
         <v>137</v>
       </c>
-      <c r="F90" s="68" t="s">
+      <c r="F90" s="67" t="s">
         <v>138</v>
       </c>
       <c r="G90" s="19" t="s">
@@ -4545,121 +4519,124 @@
       </c>
     </row>
     <row r="91" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="71" t="s">
+      <c r="A91" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="B91" s="48" t="s">
+      <c r="B91" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="C91" s="49" t="s">
+      <c r="C91" s="66" t="s">
         <v>140</v>
       </c>
-      <c r="D91" s="49">
-        <v>2</v>
-      </c>
-      <c r="E91" s="72" t="s">
+      <c r="D91" s="66">
+        <v>2</v>
+      </c>
+      <c r="E91" s="87" t="s">
         <v>141</v>
       </c>
-      <c r="F91" s="70"/>
-      <c r="G91" s="16" t="s">
+      <c r="F91" s="88"/>
+      <c r="G91" s="19" t="s">
         <v>247</v>
       </c>
-      <c r="H91" s="16"/>
-      <c r="I91" s="16"/>
-      <c r="J91" s="35" t="s">
+      <c r="H91" s="19"/>
+      <c r="I91" s="19"/>
+      <c r="J91" s="15" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="92" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="71" t="s">
+      <c r="A92" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="B92" s="48" t="s">
+      <c r="B92" s="64" t="s">
         <v>142</v>
       </c>
-      <c r="C92" s="49" t="s">
+      <c r="C92" s="66" t="s">
         <v>143</v>
       </c>
-      <c r="D92" s="49">
-        <v>2</v>
-      </c>
-      <c r="E92" s="72" t="s">
+      <c r="D92" s="66">
+        <v>2</v>
+      </c>
+      <c r="E92" s="87" t="s">
         <v>144</v>
       </c>
-      <c r="F92" s="70"/>
-      <c r="G92" s="16" t="s">
+      <c r="F92" s="88"/>
+      <c r="G92" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="H92" s="16"/>
-      <c r="I92" s="16"/>
+      <c r="H92" s="19"/>
+      <c r="I92" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="J92" s="89"/>
     </row>
     <row r="93" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="63" t="s">
+      <c r="A93" s="62" t="s">
         <v>203</v>
       </c>
-      <c r="B93" s="73" t="s">
+      <c r="B93" s="70" t="s">
         <v>145</v>
       </c>
-      <c r="C93" s="74" t="s">
+      <c r="C93" s="71" t="s">
         <v>146</v>
       </c>
-      <c r="D93" s="74">
-        <v>2</v>
-      </c>
-      <c r="E93" s="85" t="s">
+      <c r="D93" s="71">
+        <v>2</v>
+      </c>
+      <c r="E93" s="82" t="s">
         <v>147</v>
       </c>
-      <c r="F93" s="86"/>
+      <c r="F93" s="83"/>
       <c r="G93" s="24"/>
       <c r="H93" s="24"/>
       <c r="I93" s="24"/>
-      <c r="J93" s="41"/>
+      <c r="J93" s="40"/>
     </row>
     <row r="94" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A94" s="63" t="s">
+      <c r="A94" s="62" t="s">
         <v>204</v>
       </c>
-      <c r="B94" s="75" t="s">
+      <c r="B94" s="72" t="s">
         <v>148</v>
       </c>
-      <c r="C94" s="76" t="s">
+      <c r="C94" s="73" t="s">
         <v>149</v>
       </c>
-      <c r="D94" s="76">
-        <v>2</v>
-      </c>
-      <c r="E94" s="87" t="s">
+      <c r="D94" s="73">
+        <v>2</v>
+      </c>
+      <c r="E94" s="84" t="s">
         <v>150</v>
       </c>
-      <c r="F94" s="88"/>
+      <c r="F94" s="85"/>
       <c r="G94" s="24"/>
       <c r="H94" s="24"/>
       <c r="I94" s="24"/>
-      <c r="J94" s="41"/>
+      <c r="J94" s="40"/>
     </row>
     <row r="95" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="99" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B99" s="114" t="s">
+      <c r="B99" s="113" t="s">
         <v>81</v>
       </c>
-      <c r="C99" s="114"/>
-      <c r="D99" s="114"/>
-      <c r="E99" s="114"/>
-      <c r="F99" s="114"/>
+      <c r="C99" s="113"/>
+      <c r="D99" s="113"/>
+      <c r="E99" s="113"/>
+      <c r="F99" s="113"/>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B100" s="114"/>
-      <c r="C100" s="114"/>
-      <c r="D100" s="114"/>
-      <c r="E100" s="114"/>
-      <c r="F100" s="114"/>
+      <c r="B100" s="113"/>
+      <c r="C100" s="113"/>
+      <c r="D100" s="113"/>
+      <c r="E100" s="113"/>
+      <c r="F100" s="113"/>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B101" s="114"/>
-      <c r="C101" s="114"/>
-      <c r="D101" s="114"/>
-      <c r="E101" s="114"/>
-      <c r="F101" s="114"/>
+      <c r="B101" s="113"/>
+      <c r="C101" s="113"/>
+      <c r="D101" s="113"/>
+      <c r="E101" s="113"/>
+      <c r="F101" s="113"/>
     </row>
     <row r="128" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C128" t="s">
@@ -4676,24 +4653,24 @@
     </row>
     <row r="132" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="133" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B133" s="102" t="s">
+      <c r="B133" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="C133" s="103"/>
+      <c r="C133" s="108"/>
       <c r="D133" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E133" s="104" t="s">
-        <v>2</v>
-      </c>
-      <c r="F133" s="105"/>
-      <c r="G133" s="69" t="s">
+      <c r="E133" s="109" t="s">
+        <v>2</v>
+      </c>
+      <c r="F133" s="110"/>
+      <c r="G133" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="H133" s="69" t="s">
+      <c r="H133" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="I133" s="69" t="s">
+      <c r="I133" s="68" t="s">
         <v>26</v>
       </c>
     </row>
@@ -4705,8 +4682,8 @@
         <v>4</v>
       </c>
       <c r="D134" s="5"/>
-      <c r="E134" s="106"/>
-      <c r="F134" s="107"/>
+      <c r="E134" s="111"/>
+      <c r="F134" s="112"/>
       <c r="G134" s="16"/>
       <c r="H134" s="16" t="s">
         <v>215</v>
@@ -4729,7 +4706,7 @@
       <c r="F135" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G135" s="53" t="s">
+      <c r="G135" s="52" t="s">
         <v>25</v>
       </c>
       <c r="H135" s="17" t="s">
@@ -4753,7 +4730,7 @@
       <c r="F136" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G136" s="53">
+      <c r="G136" s="52">
         <v>30</v>
       </c>
       <c r="H136" s="17" t="s">
@@ -4773,10 +4750,10 @@
       <c r="D137" s="9">
         <v>2</v>
       </c>
-      <c r="E137" s="108" t="s">
+      <c r="E137" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="F137" s="109"/>
+      <c r="F137" s="102"/>
       <c r="G137" s="16" t="s">
         <v>218</v>
       </c>
@@ -4797,10 +4774,10 @@
       <c r="D138" s="9">
         <v>3</v>
       </c>
-      <c r="E138" s="101" t="s">
+      <c r="E138" s="99" t="s">
         <v>63</v>
       </c>
-      <c r="F138" s="95"/>
+      <c r="F138" s="100"/>
       <c r="G138" s="16" t="s">
         <v>221</v>
       </c>
@@ -4819,10 +4796,10 @@
       <c r="D139" s="9">
         <v>2</v>
       </c>
-      <c r="E139" s="101" t="s">
+      <c r="E139" s="99" t="s">
         <v>64</v>
       </c>
-      <c r="F139" s="95"/>
+      <c r="F139" s="100"/>
       <c r="G139" s="16" t="s">
         <v>223</v>
       </c>
@@ -4841,10 +4818,10 @@
       <c r="D140" s="9">
         <v>2</v>
       </c>
-      <c r="E140" s="101" t="s">
+      <c r="E140" s="99" t="s">
         <v>65</v>
       </c>
-      <c r="F140" s="95"/>
+      <c r="F140" s="100"/>
       <c r="G140" s="16"/>
       <c r="H140" s="16"/>
       <c r="I140" s="16"/>
@@ -4859,10 +4836,10 @@
       <c r="D141" s="9">
         <v>1</v>
       </c>
-      <c r="E141" s="101" t="s">
+      <c r="E141" s="99" t="s">
         <v>66</v>
       </c>
-      <c r="F141" s="95"/>
+      <c r="F141" s="100"/>
       <c r="G141" s="16"/>
       <c r="H141" s="16"/>
       <c r="I141" s="16"/>
@@ -4877,10 +4854,10 @@
       <c r="D142" s="9">
         <v>2</v>
       </c>
-      <c r="E142" s="101" t="s">
+      <c r="E142" s="99" t="s">
         <v>67</v>
       </c>
-      <c r="F142" s="95"/>
+      <c r="F142" s="100"/>
       <c r="G142" s="16"/>
       <c r="H142" s="16"/>
       <c r="I142" s="16"/>
@@ -4895,10 +4872,10 @@
       <c r="D143" s="9">
         <v>1</v>
       </c>
-      <c r="E143" s="101" t="s">
+      <c r="E143" s="99" t="s">
         <v>68</v>
       </c>
-      <c r="F143" s="95"/>
+      <c r="F143" s="100"/>
       <c r="G143" s="16"/>
       <c r="H143" s="16"/>
       <c r="I143" s="16"/>
@@ -4913,10 +4890,10 @@
       <c r="D144" s="9">
         <v>4</v>
       </c>
-      <c r="E144" s="101" t="s">
+      <c r="E144" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="F144" s="95"/>
+      <c r="F144" s="100"/>
       <c r="G144" s="16" t="s">
         <v>216</v>
       </c>
@@ -4933,10 +4910,10 @@
       <c r="D145" s="9">
         <v>1</v>
       </c>
-      <c r="E145" s="36" t="s">
+      <c r="E145" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="F145" s="36" t="s">
+      <c r="F145" s="35" t="s">
         <v>70</v>
       </c>
       <c r="G145" s="16"/>
@@ -4953,10 +4930,10 @@
       <c r="D146" s="9">
         <v>2</v>
       </c>
-      <c r="E146" s="101" t="s">
+      <c r="E146" s="99" t="s">
         <v>71</v>
       </c>
-      <c r="F146" s="95"/>
+      <c r="F146" s="100"/>
       <c r="G146" s="16"/>
       <c r="H146" s="16"/>
       <c r="I146" s="16"/>
@@ -4971,10 +4948,10 @@
       <c r="D147" s="9">
         <v>2</v>
       </c>
-      <c r="E147" s="101" t="s">
+      <c r="E147" s="99" t="s">
         <v>72</v>
       </c>
-      <c r="F147" s="95"/>
+      <c r="F147" s="100"/>
       <c r="G147" s="16"/>
       <c r="H147" s="16"/>
       <c r="I147" s="16"/>
@@ -4989,10 +4966,10 @@
       <c r="D148" s="9">
         <v>2</v>
       </c>
-      <c r="E148" s="101" t="s">
+      <c r="E148" s="99" t="s">
         <v>73</v>
       </c>
-      <c r="F148" s="95"/>
+      <c r="F148" s="100"/>
       <c r="G148" s="16"/>
       <c r="H148" s="16"/>
       <c r="I148" s="16"/>
@@ -5007,10 +4984,10 @@
       <c r="D149" s="9">
         <v>2</v>
       </c>
-      <c r="E149" s="101" t="s">
+      <c r="E149" s="99" t="s">
         <v>74</v>
       </c>
-      <c r="F149" s="95"/>
+      <c r="F149" s="100"/>
       <c r="G149" s="16"/>
       <c r="H149" s="16"/>
       <c r="I149" s="16"/>
@@ -5025,10 +5002,10 @@
       <c r="D150" s="9">
         <v>4</v>
       </c>
-      <c r="E150" s="101" t="s">
+      <c r="E150" s="99" t="s">
         <v>75</v>
       </c>
-      <c r="F150" s="95"/>
+      <c r="F150" s="100"/>
       <c r="G150" s="16"/>
       <c r="H150" s="16"/>
       <c r="I150" s="16"/>
@@ -5043,10 +5020,10 @@
       <c r="D151" s="9">
         <v>4</v>
       </c>
-      <c r="E151" s="101" t="s">
+      <c r="E151" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="F151" s="95"/>
+      <c r="F151" s="100"/>
       <c r="G151" s="16"/>
       <c r="H151" s="16"/>
       <c r="I151" s="16"/>
@@ -5061,10 +5038,10 @@
       <c r="D152" s="9">
         <v>2</v>
       </c>
-      <c r="E152" s="101" t="s">
+      <c r="E152" s="99" t="s">
         <v>77</v>
       </c>
-      <c r="F152" s="95"/>
+      <c r="F152" s="100"/>
       <c r="G152" s="16"/>
       <c r="H152" s="16"/>
       <c r="I152" s="16"/>
@@ -5079,10 +5056,10 @@
       <c r="D153" s="9">
         <v>2</v>
       </c>
-      <c r="E153" s="101" t="s">
+      <c r="E153" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="F153" s="95"/>
+      <c r="F153" s="100"/>
       <c r="G153" s="16"/>
       <c r="H153" s="16"/>
       <c r="I153" s="16"/>
@@ -5097,10 +5074,10 @@
       <c r="D154" s="9">
         <v>8</v>
       </c>
-      <c r="E154" s="101" t="s">
+      <c r="E154" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="F154" s="95"/>
+      <c r="F154" s="100"/>
       <c r="G154" s="16"/>
       <c r="H154" s="16"/>
       <c r="I154" s="16"/>
@@ -5115,10 +5092,10 @@
       <c r="D155" s="9">
         <v>4</v>
       </c>
-      <c r="E155" s="101" t="s">
+      <c r="E155" s="99" t="s">
         <v>79</v>
       </c>
-      <c r="F155" s="95"/>
+      <c r="F155" s="100"/>
       <c r="G155" s="16"/>
       <c r="H155" s="16"/>
       <c r="I155" s="16"/>
@@ -5133,10 +5110,10 @@
       <c r="D156" s="9">
         <v>4</v>
       </c>
-      <c r="E156" s="101" t="s">
+      <c r="E156" s="99" t="s">
         <v>80</v>
       </c>
-      <c r="F156" s="95"/>
+      <c r="F156" s="100"/>
       <c r="G156" s="16"/>
       <c r="H156" s="16"/>
       <c r="I156" s="16"/>

</xml_diff>